<commit_message>
Removed html tags and hyperlink from study_search in aact_table
</commit_message>
<xml_diff>
--- a/public/documentation/aact_beta_tables.xlsx
+++ b/public/documentation/aact_beta_tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abykova/Projects/aact-admin/public/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEB4763-116F-B44E-BAD4-C277B5A3FD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E35B64-B886-B94C-AA3E-EDDE90B9FD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32820" yWindow="-1840" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1257,27 +1257,6 @@
     <t>study_searches</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">These are saved queries that are used to search </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="12"/>
-        <color rgb="FF1155CC"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ClinicalTrials.gov</t>
-    </r>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
@@ -1381,12 +1360,15 @@
   <si>
     <t>It contains the total count of people effected by reported events grouped by the type of event</t>
   </si>
+  <si>
+    <t>These are saved queries that are used to search ClinicalTrials.gov</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1432,13 +1414,6 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
@@ -1448,13 +1423,6 @@
       <u/>
       <sz val="12"/>
       <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF1155CC"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1551,13 +1519,10 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1569,12 +1534,13 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1848,8 +1814,8 @@
       <c r="Z1" s="4"/>
     </row>
     <row r="2" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="23" t="s">
-        <v>160</v>
+      <c r="A2" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
@@ -1888,8 +1854,8 @@
       <c r="Z2" s="4"/>
     </row>
     <row r="3" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="23" t="s">
-        <v>160</v>
+      <c r="A3" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>11</v>
@@ -1928,8 +1894,8 @@
       <c r="Z3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="23" t="s">
-        <v>160</v>
+      <c r="A4" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>14</v>
@@ -1968,8 +1934,8 @@
       <c r="Z4" s="4"/>
     </row>
     <row r="5" spans="1:26" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="23" t="s">
-        <v>160</v>
+      <c r="A5" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>19</v>
@@ -2006,8 +1972,8 @@
       <c r="Z5" s="4"/>
     </row>
     <row r="6" spans="1:26" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="23" t="s">
-        <v>160</v>
+      <c r="A6" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>21</v>
@@ -2044,8 +2010,8 @@
       <c r="Z6" s="4"/>
     </row>
     <row r="7" spans="1:26" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="23" t="s">
-        <v>160</v>
+      <c r="A7" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>23</v>
@@ -2082,8 +2048,8 @@
       <c r="Z7" s="4"/>
     </row>
     <row r="8" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
-        <v>160</v>
+      <c r="A8" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>25</v>
@@ -2122,8 +2088,8 @@
       <c r="Z8" s="4"/>
     </row>
     <row r="9" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="23" t="s">
-        <v>160</v>
+      <c r="A9" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>28</v>
@@ -2162,8 +2128,8 @@
       <c r="Z9" s="4"/>
     </row>
     <row r="10" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="23" t="s">
-        <v>160</v>
+      <c r="A10" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>30</v>
@@ -2202,8 +2168,8 @@
       <c r="Z10" s="4"/>
     </row>
     <row r="11" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="23" t="s">
-        <v>160</v>
+      <c r="A11" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>32</v>
@@ -2242,8 +2208,8 @@
       <c r="Z11" s="4"/>
     </row>
     <row r="12" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="23" t="s">
-        <v>160</v>
+      <c r="A12" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>35</v>
@@ -2282,8 +2248,8 @@
       <c r="Z12" s="4"/>
     </row>
     <row r="13" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="23" t="s">
-        <v>160</v>
+      <c r="A13" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>38</v>
@@ -2322,8 +2288,8 @@
       <c r="Z13" s="4"/>
     </row>
     <row r="14" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="23" t="s">
-        <v>160</v>
+      <c r="A14" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>41</v>
@@ -2362,8 +2328,8 @@
       <c r="Z14" s="4"/>
     </row>
     <row r="15" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="23" t="s">
-        <v>160</v>
+      <c r="A15" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>44</v>
@@ -2402,8 +2368,8 @@
       <c r="Z15" s="4"/>
     </row>
     <row r="16" spans="1:26" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
-        <v>160</v>
+      <c r="A16" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>47</v>
@@ -2442,8 +2408,8 @@
       <c r="Z16" s="4"/>
     </row>
     <row r="17" spans="1:26" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="23" t="s">
-        <v>160</v>
+      <c r="A17" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>50</v>
@@ -2482,8 +2448,8 @@
       <c r="Z17" s="4"/>
     </row>
     <row r="18" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="23" t="s">
-        <v>160</v>
+      <c r="A18" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>53</v>
@@ -2522,8 +2488,8 @@
       <c r="Z18" s="4"/>
     </row>
     <row r="19" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="23" t="s">
-        <v>160</v>
+      <c r="A19" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>56</v>
@@ -2562,8 +2528,8 @@
       <c r="Z19" s="4"/>
     </row>
     <row r="20" spans="1:26" ht="153" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="23" t="s">
-        <v>160</v>
+      <c r="A20" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>59</v>
@@ -2602,8 +2568,8 @@
       <c r="Z20" s="4"/>
     </row>
     <row r="21" spans="1:26" ht="135.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="23" t="s">
-        <v>160</v>
+      <c r="A21" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>62</v>
@@ -2642,8 +2608,8 @@
       <c r="Z21" s="4"/>
     </row>
     <row r="22" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="23" t="s">
-        <v>160</v>
+      <c r="A22" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>65</v>
@@ -2682,8 +2648,8 @@
       <c r="Z22" s="4"/>
     </row>
     <row r="23" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="23" t="s">
-        <v>160</v>
+      <c r="A23" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>68</v>
@@ -2722,8 +2688,8 @@
       <c r="Z23" s="4"/>
     </row>
     <row r="24" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="23" t="s">
-        <v>160</v>
+      <c r="A24" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>71</v>
@@ -2762,8 +2728,8 @@
       <c r="Z24" s="4"/>
     </row>
     <row r="25" spans="1:26" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="23" t="s">
-        <v>160</v>
+      <c r="A25" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>74</v>
@@ -2802,8 +2768,8 @@
       <c r="Z25" s="4"/>
     </row>
     <row r="26" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="23" t="s">
-        <v>160</v>
+      <c r="A26" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>77</v>
@@ -2842,8 +2808,8 @@
       <c r="Z26" s="4"/>
     </row>
     <row r="27" spans="1:26" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="23" t="s">
-        <v>160</v>
+      <c r="A27" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>80</v>
@@ -2882,8 +2848,8 @@
       <c r="Z27" s="4"/>
     </row>
     <row r="28" spans="1:26" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="23" t="s">
-        <v>160</v>
+      <c r="A28" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>83</v>
@@ -2922,8 +2888,8 @@
       <c r="Z28" s="4"/>
     </row>
     <row r="29" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="23" t="s">
-        <v>160</v>
+      <c r="A29" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>86</v>
@@ -2962,8 +2928,8 @@
       <c r="Z29" s="4"/>
     </row>
     <row r="30" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="23" t="s">
-        <v>160</v>
+      <c r="A30" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>89</v>
@@ -3002,8 +2968,8 @@
       <c r="Z30" s="4"/>
     </row>
     <row r="31" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="23" t="s">
-        <v>160</v>
+      <c r="A31" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>92</v>
@@ -3042,8 +3008,8 @@
       <c r="Z31" s="4"/>
     </row>
     <row r="32" spans="1:26" ht="84.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="23" t="s">
-        <v>160</v>
+      <c r="A32" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>95</v>
@@ -3082,8 +3048,8 @@
       <c r="Z32" s="4"/>
     </row>
     <row r="33" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="23" t="s">
-        <v>160</v>
+      <c r="A33" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>98</v>
@@ -3122,8 +3088,8 @@
       <c r="Z33" s="4"/>
     </row>
     <row r="34" spans="1:26" ht="84.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="23" t="s">
-        <v>160</v>
+      <c r="A34" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>101</v>
@@ -3162,8 +3128,8 @@
       <c r="Z34" s="4"/>
     </row>
     <row r="35" spans="1:26" ht="81" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="23" t="s">
-        <v>160</v>
+      <c r="A35" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>104</v>
@@ -3200,8 +3166,8 @@
       <c r="Z35" s="4"/>
     </row>
     <row r="36" spans="1:26" ht="81" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="23" t="s">
-        <v>160</v>
+      <c r="A36" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>106</v>
@@ -3240,8 +3206,8 @@
       <c r="Z36" s="4"/>
     </row>
     <row r="37" spans="1:26" ht="70" x14ac:dyDescent="0.15">
-      <c r="A37" s="23" t="s">
-        <v>160</v>
+      <c r="A37" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B37" s="5" t="s">
         <v>109</v>
@@ -3280,26 +3246,26 @@
       <c r="Z37" s="4"/>
     </row>
     <row r="38" spans="1:26" s="4" customFormat="1" ht="28" x14ac:dyDescent="0.15">
-      <c r="A38" s="23" t="s">
+      <c r="A38" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C38" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="D38" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="1:26" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="22" t="s">
         <v>159</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="D38" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" s="6"/>
-    </row>
-    <row r="39" spans="1:26" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="23" t="s">
-        <v>160</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>112</v>
@@ -3338,8 +3304,8 @@
       <c r="Z39" s="4"/>
     </row>
     <row r="40" spans="1:26" ht="84.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="23" t="s">
-        <v>160</v>
+      <c r="A40" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>115</v>
@@ -3378,8 +3344,8 @@
       <c r="Z40" s="4"/>
     </row>
     <row r="41" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="23" t="s">
-        <v>160</v>
+      <c r="A41" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>118</v>
@@ -3418,8 +3384,8 @@
       <c r="Z41" s="4"/>
     </row>
     <row r="42" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="23" t="s">
-        <v>160</v>
+      <c r="A42" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>121</v>
@@ -3458,8 +3424,8 @@
       <c r="Z42" s="4"/>
     </row>
     <row r="43" spans="1:26" ht="34" x14ac:dyDescent="0.2">
-      <c r="A43" s="23" t="s">
-        <v>160</v>
+      <c r="A43" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B43" s="14" t="s">
         <v>124</v>
@@ -3498,8 +3464,8 @@
       <c r="Z43" s="4"/>
     </row>
     <row r="44" spans="1:26" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="23" t="s">
-        <v>160</v>
+      <c r="A44" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>127</v>
@@ -3538,8 +3504,8 @@
       <c r="Z44" s="4"/>
     </row>
     <row r="45" spans="1:26" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="23" t="s">
-        <v>160</v>
+      <c r="A45" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>130</v>
@@ -3576,8 +3542,8 @@
       <c r="Z45" s="4"/>
     </row>
     <row r="46" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="23" t="s">
-        <v>160</v>
+      <c r="A46" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>133</v>
@@ -3614,17 +3580,17 @@
       <c r="Z46" s="4"/>
     </row>
     <row r="47" spans="1:26" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="23" t="s">
-        <v>160</v>
+      <c r="A47" s="22" t="s">
+        <v>159</v>
       </c>
       <c r="B47" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="C47" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="D47" s="14" t="s">
         <v>136</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>137</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>126</v>
@@ -3655,21 +3621,21 @@
     </row>
     <row r="48" spans="1:26" ht="84.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="C48" s="2" t="s">
         <v>139</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>140</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>126</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F48" s="17"/>
+        <v>140</v>
+      </c>
+      <c r="F48" s="16"/>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
@@ -3693,21 +3659,21 @@
     </row>
     <row r="49" spans="1:26" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>126</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F49" s="17"/>
+        <v>140</v>
+      </c>
+      <c r="F49" s="16"/>
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
@@ -3731,21 +3697,21 @@
     </row>
     <row r="50" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>126</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F50" s="17"/>
+        <v>140</v>
+      </c>
+      <c r="F50" s="16"/>
       <c r="G50" s="4"/>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
@@ -3769,21 +3735,21 @@
     </row>
     <row r="51" spans="1:26" ht="51" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B51" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>147</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>148</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>126</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F51" s="17"/>
+        <v>140</v>
+      </c>
+      <c r="F51" s="16"/>
       <c r="G51" s="4"/>
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
@@ -3807,21 +3773,21 @@
     </row>
     <row r="52" spans="1:26" ht="84.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C52" s="17" t="s">
         <v>149</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C52" s="18" t="s">
-        <v>150</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>126</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F52" s="19"/>
+        <v>140</v>
+      </c>
+      <c r="F52" s="18"/>
       <c r="G52" s="4"/>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
@@ -3845,21 +3811,21 @@
     </row>
     <row r="53" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="17" t="s">
         <v>152</v>
-      </c>
-      <c r="C53" s="18" t="s">
-        <v>153</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>126</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F53" s="19"/>
+        <v>140</v>
+      </c>
+      <c r="F53" s="18"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
@@ -3883,21 +3849,21 @@
     </row>
     <row r="54" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C54" s="17" t="s">
         <v>154</v>
-      </c>
-      <c r="C54" s="18" t="s">
-        <v>155</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>126</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F54" s="17"/>
+        <v>140</v>
+      </c>
+      <c r="F54" s="16"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
@@ -3921,21 +3887,21 @@
     </row>
     <row r="55" spans="1:26" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C55" s="17" t="s">
         <v>156</v>
-      </c>
-      <c r="C55" s="18" t="s">
-        <v>157</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>126</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F55" s="17"/>
+        <v>140</v>
+      </c>
+      <c r="F55" s="16"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
@@ -3959,21 +3925,21 @@
     </row>
     <row r="56" spans="1:26" ht="84.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>126</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F56" s="17"/>
+        <v>140</v>
+      </c>
+      <c r="F56" s="16"/>
       <c r="G56" s="4"/>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
@@ -3996,12 +3962,12 @@
       <c r="Z56" s="4"/>
     </row>
     <row r="57" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="20"/>
-      <c r="B57" s="20"/>
-      <c r="C57" s="19"/>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="17"/>
+      <c r="A57" s="19"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="16"/>
       <c r="G57" s="4"/>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
@@ -4024,12 +3990,12 @@
       <c r="Z57" s="4"/>
     </row>
     <row r="58" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="20"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="19"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="20"/>
-      <c r="F58" s="17"/>
+      <c r="A58" s="19"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="18"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="19"/>
+      <c r="F58" s="16"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
@@ -4052,12 +4018,12 @@
       <c r="Z58" s="4"/>
     </row>
     <row r="59" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="20"/>
-      <c r="B59" s="20"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="20"/>
-      <c r="E59" s="20"/>
-      <c r="F59" s="17"/>
+      <c r="A59" s="19"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="19"/>
+      <c r="E59" s="19"/>
+      <c r="F59" s="16"/>
       <c r="G59" s="4"/>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
@@ -4080,12 +4046,12 @@
       <c r="Z59" s="4"/>
     </row>
     <row r="60" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="20"/>
-      <c r="B60" s="20"/>
-      <c r="C60" s="19"/>
-      <c r="D60" s="20"/>
-      <c r="E60" s="20"/>
-      <c r="F60" s="17"/>
+      <c r="A60" s="19"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="16"/>
       <c r="G60" s="4"/>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
@@ -4108,12 +4074,12 @@
       <c r="Z60" s="4"/>
     </row>
     <row r="61" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="20"/>
-      <c r="B61" s="20"/>
-      <c r="C61" s="19"/>
-      <c r="D61" s="20"/>
-      <c r="E61" s="20"/>
-      <c r="F61" s="17"/>
+      <c r="A61" s="19"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="18"/>
+      <c r="D61" s="19"/>
+      <c r="E61" s="19"/>
+      <c r="F61" s="16"/>
       <c r="G61" s="4"/>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
@@ -4136,12 +4102,12 @@
       <c r="Z61" s="4"/>
     </row>
     <row r="62" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="20"/>
-      <c r="B62" s="20"/>
-      <c r="C62" s="19"/>
-      <c r="D62" s="20"/>
-      <c r="E62" s="20"/>
-      <c r="F62" s="17"/>
+      <c r="A62" s="19"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="18"/>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="16"/>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
@@ -4164,12 +4130,12 @@
       <c r="Z62" s="4"/>
     </row>
     <row r="63" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="20"/>
-      <c r="B63" s="20"/>
-      <c r="C63" s="19"/>
-      <c r="D63" s="20"/>
-      <c r="E63" s="20"/>
-      <c r="F63" s="17"/>
+      <c r="A63" s="19"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19"/>
+      <c r="F63" s="16"/>
       <c r="G63" s="4"/>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
@@ -4192,12 +4158,12 @@
       <c r="Z63" s="4"/>
     </row>
     <row r="64" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="20"/>
-      <c r="B64" s="20"/>
-      <c r="C64" s="19"/>
-      <c r="D64" s="19"/>
-      <c r="E64" s="20"/>
-      <c r="F64" s="19"/>
+      <c r="A64" s="19"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="19"/>
+      <c r="F64" s="18"/>
       <c r="G64" s="4"/>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
@@ -4220,12 +4186,12 @@
       <c r="Z64" s="4"/>
     </row>
     <row r="65" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="20"/>
-      <c r="B65" s="20"/>
-      <c r="C65" s="19"/>
-      <c r="D65" s="19"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="19"/>
+      <c r="A65" s="19"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="18"/>
+      <c r="D65" s="18"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="18"/>
       <c r="G65" s="4"/>
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
@@ -4248,12 +4214,12 @@
       <c r="Z65" s="4"/>
     </row>
     <row r="66" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="20"/>
-      <c r="B66" s="20"/>
-      <c r="C66" s="19"/>
-      <c r="D66" s="19"/>
-      <c r="E66" s="20"/>
-      <c r="F66" s="19"/>
+      <c r="A66" s="19"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="18"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="18"/>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
@@ -4276,12 +4242,12 @@
       <c r="Z66" s="4"/>
     </row>
     <row r="67" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="20"/>
-      <c r="B67" s="20"/>
-      <c r="C67" s="19"/>
-      <c r="D67" s="20"/>
-      <c r="E67" s="20"/>
-      <c r="F67" s="17"/>
+      <c r="A67" s="19"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="18"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="16"/>
       <c r="G67" s="4"/>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
@@ -4304,12 +4270,12 @@
       <c r="Z67" s="4"/>
     </row>
     <row r="68" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="20"/>
-      <c r="B68" s="20"/>
-      <c r="C68" s="19"/>
-      <c r="D68" s="20"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="17"/>
+      <c r="A68" s="19"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="16"/>
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
@@ -4332,12 +4298,12 @@
       <c r="Z68" s="4"/>
     </row>
     <row r="69" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="20"/>
-      <c r="B69" s="20"/>
-      <c r="C69" s="19"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="17"/>
+      <c r="A69" s="19"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="16"/>
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
       <c r="I69" s="4"/>
@@ -4360,12 +4326,12 @@
       <c r="Z69" s="4"/>
     </row>
     <row r="70" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="20"/>
-      <c r="B70" s="20"/>
-      <c r="C70" s="19"/>
-      <c r="D70" s="20"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="17"/>
+      <c r="A70" s="19"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="19"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="16"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
@@ -4388,12 +4354,12 @@
       <c r="Z70" s="4"/>
     </row>
     <row r="71" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="20"/>
-      <c r="B71" s="20"/>
-      <c r="C71" s="19"/>
-      <c r="D71" s="20"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="17"/>
+      <c r="A71" s="19"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="16"/>
       <c r="G71" s="4"/>
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
@@ -4416,12 +4382,12 @@
       <c r="Z71" s="4"/>
     </row>
     <row r="72" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="20"/>
-      <c r="B72" s="20"/>
-      <c r="C72" s="19"/>
-      <c r="D72" s="20"/>
-      <c r="E72" s="20"/>
-      <c r="F72" s="17"/>
+      <c r="A72" s="19"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="19"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="16"/>
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
@@ -4444,12 +4410,12 @@
       <c r="Z72" s="4"/>
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="20"/>
-      <c r="B73" s="20"/>
-      <c r="C73" s="19"/>
-      <c r="D73" s="19"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="19"/>
+      <c r="A73" s="19"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="18"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="18"/>
       <c r="G73" s="4"/>
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
@@ -4472,12 +4438,12 @@
       <c r="Z73" s="4"/>
     </row>
     <row r="74" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="20"/>
-      <c r="B74" s="20"/>
-      <c r="C74" s="19"/>
-      <c r="D74" s="19"/>
-      <c r="E74" s="20"/>
-      <c r="F74" s="19"/>
+      <c r="A74" s="19"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="18"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="18"/>
       <c r="G74" s="4"/>
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
@@ -4500,12 +4466,12 @@
       <c r="Z74" s="4"/>
     </row>
     <row r="75" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="20"/>
-      <c r="B75" s="20"/>
-      <c r="C75" s="19"/>
-      <c r="D75" s="20"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="17"/>
+      <c r="A75" s="19"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="16"/>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
@@ -4528,12 +4494,12 @@
       <c r="Z75" s="4"/>
     </row>
     <row r="76" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="20"/>
-      <c r="B76" s="20"/>
-      <c r="C76" s="19"/>
-      <c r="D76" s="20"/>
-      <c r="E76" s="20"/>
-      <c r="F76" s="17"/>
+      <c r="A76" s="19"/>
+      <c r="B76" s="19"/>
+      <c r="C76" s="18"/>
+      <c r="D76" s="19"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="16"/>
       <c r="G76" s="4"/>
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
@@ -4556,12 +4522,12 @@
       <c r="Z76" s="4"/>
     </row>
     <row r="77" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="20"/>
-      <c r="B77" s="20"/>
-      <c r="C77" s="19"/>
-      <c r="D77" s="20"/>
-      <c r="E77" s="20"/>
-      <c r="F77" s="17"/>
+      <c r="A77" s="19"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="19"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="16"/>
       <c r="G77" s="4"/>
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
@@ -4584,12 +4550,12 @@
       <c r="Z77" s="4"/>
     </row>
     <row r="78" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="20"/>
-      <c r="B78" s="20"/>
-      <c r="C78" s="19"/>
-      <c r="D78" s="19"/>
-      <c r="E78" s="20"/>
-      <c r="F78" s="19"/>
+      <c r="A78" s="19"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="18"/>
+      <c r="D78" s="18"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="18"/>
       <c r="G78" s="4"/>
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
@@ -4612,12 +4578,12 @@
       <c r="Z78" s="4"/>
     </row>
     <row r="79" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="20"/>
-      <c r="B79" s="20"/>
-      <c r="C79" s="19"/>
-      <c r="D79" s="20"/>
-      <c r="E79" s="20"/>
-      <c r="F79" s="17"/>
+      <c r="A79" s="19"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="19"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="16"/>
       <c r="G79" s="4"/>
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
@@ -4640,12 +4606,12 @@
       <c r="Z79" s="4"/>
     </row>
     <row r="80" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="20"/>
-      <c r="B80" s="20"/>
-      <c r="C80" s="19"/>
-      <c r="D80" s="20"/>
-      <c r="E80" s="20"/>
-      <c r="F80" s="17"/>
+      <c r="A80" s="19"/>
+      <c r="B80" s="19"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="19"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="16"/>
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
@@ -4668,12 +4634,12 @@
       <c r="Z80" s="4"/>
     </row>
     <row r="81" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="20"/>
-      <c r="B81" s="20"/>
-      <c r="C81" s="19"/>
-      <c r="D81" s="20"/>
-      <c r="E81" s="20"/>
-      <c r="F81" s="17"/>
+      <c r="A81" s="19"/>
+      <c r="B81" s="19"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="19"/>
+      <c r="E81" s="19"/>
+      <c r="F81" s="16"/>
       <c r="G81" s="4"/>
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
@@ -4696,12 +4662,12 @@
       <c r="Z81" s="4"/>
     </row>
     <row r="82" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="20"/>
-      <c r="B82" s="20"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="19"/>
-      <c r="E82" s="20"/>
-      <c r="F82" s="17"/>
+      <c r="A82" s="19"/>
+      <c r="B82" s="19"/>
+      <c r="C82" s="18"/>
+      <c r="D82" s="18"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="16"/>
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
@@ -4724,12 +4690,12 @@
       <c r="Z82" s="4"/>
     </row>
     <row r="83" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="20"/>
-      <c r="B83" s="20"/>
-      <c r="C83" s="19"/>
-      <c r="D83" s="19"/>
-      <c r="E83" s="20"/>
-      <c r="F83" s="17"/>
+      <c r="A83" s="19"/>
+      <c r="B83" s="19"/>
+      <c r="C83" s="18"/>
+      <c r="D83" s="18"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="16"/>
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
@@ -4752,12 +4718,12 @@
       <c r="Z83" s="4"/>
     </row>
     <row r="84" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="20"/>
-      <c r="B84" s="20"/>
-      <c r="C84" s="19"/>
-      <c r="D84" s="19"/>
-      <c r="E84" s="20"/>
-      <c r="F84" s="17"/>
+      <c r="A84" s="19"/>
+      <c r="B84" s="19"/>
+      <c r="C84" s="18"/>
+      <c r="D84" s="18"/>
+      <c r="E84" s="19"/>
+      <c r="F84" s="16"/>
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
@@ -4780,12 +4746,12 @@
       <c r="Z84" s="4"/>
     </row>
     <row r="85" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="20"/>
-      <c r="B85" s="20"/>
-      <c r="C85" s="19"/>
-      <c r="D85" s="19"/>
-      <c r="E85" s="20"/>
-      <c r="F85" s="17"/>
+      <c r="A85" s="19"/>
+      <c r="B85" s="19"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="18"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="16"/>
       <c r="G85" s="4"/>
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
@@ -4808,12 +4774,12 @@
       <c r="Z85" s="4"/>
     </row>
     <row r="86" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A86" s="20"/>
-      <c r="B86" s="20"/>
-      <c r="C86" s="19"/>
-      <c r="D86" s="19"/>
-      <c r="E86" s="20"/>
-      <c r="F86" s="17"/>
+      <c r="A86" s="19"/>
+      <c r="B86" s="19"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="18"/>
+      <c r="E86" s="19"/>
+      <c r="F86" s="16"/>
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
       <c r="I86" s="4"/>
@@ -4836,12 +4802,12 @@
       <c r="Z86" s="4"/>
     </row>
     <row r="87" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="20"/>
-      <c r="B87" s="20"/>
-      <c r="C87" s="19"/>
-      <c r="D87" s="19"/>
-      <c r="E87" s="20"/>
-      <c r="F87" s="17"/>
+      <c r="A87" s="19"/>
+      <c r="B87" s="19"/>
+      <c r="C87" s="18"/>
+      <c r="D87" s="18"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="16"/>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
@@ -4864,12 +4830,12 @@
       <c r="Z87" s="4"/>
     </row>
     <row r="88" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="20"/>
-      <c r="B88" s="20"/>
-      <c r="C88" s="19"/>
-      <c r="D88" s="19"/>
-      <c r="E88" s="20"/>
-      <c r="F88" s="17"/>
+      <c r="A88" s="19"/>
+      <c r="B88" s="19"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="18"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="16"/>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
@@ -4892,12 +4858,12 @@
       <c r="Z88" s="4"/>
     </row>
     <row r="89" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="20"/>
-      <c r="B89" s="20"/>
-      <c r="C89" s="19"/>
-      <c r="D89" s="19"/>
-      <c r="E89" s="20"/>
-      <c r="F89" s="17"/>
+      <c r="A89" s="19"/>
+      <c r="B89" s="19"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="18"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="16"/>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
@@ -4920,12 +4886,12 @@
       <c r="Z89" s="4"/>
     </row>
     <row r="90" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A90" s="20"/>
-      <c r="B90" s="20"/>
-      <c r="C90" s="21"/>
-      <c r="D90" s="21"/>
-      <c r="E90" s="20"/>
-      <c r="F90" s="19"/>
+      <c r="A90" s="19"/>
+      <c r="B90" s="19"/>
+      <c r="C90" s="20"/>
+      <c r="D90" s="20"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="18"/>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
@@ -4948,12 +4914,12 @@
       <c r="Z90" s="4"/>
     </row>
     <row r="91" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="20"/>
-      <c r="B91" s="20"/>
-      <c r="C91" s="19"/>
-      <c r="D91" s="19"/>
-      <c r="E91" s="20"/>
-      <c r="F91" s="17"/>
+      <c r="A91" s="19"/>
+      <c r="B91" s="19"/>
+      <c r="C91" s="18"/>
+      <c r="D91" s="18"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="16"/>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
@@ -4976,12 +4942,12 @@
       <c r="Z91" s="4"/>
     </row>
     <row r="92" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="20"/>
-      <c r="B92" s="20"/>
-      <c r="C92" s="21"/>
-      <c r="D92" s="21"/>
-      <c r="E92" s="20"/>
-      <c r="F92" s="19"/>
+      <c r="A92" s="19"/>
+      <c r="B92" s="19"/>
+      <c r="C92" s="20"/>
+      <c r="D92" s="20"/>
+      <c r="E92" s="19"/>
+      <c r="F92" s="18"/>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
       <c r="I92" s="4"/>
@@ -5004,12 +4970,12 @@
       <c r="Z92" s="4"/>
     </row>
     <row r="93" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="20"/>
-      <c r="B93" s="20"/>
-      <c r="C93" s="21"/>
-      <c r="D93" s="21"/>
-      <c r="E93" s="20"/>
-      <c r="F93" s="19"/>
+      <c r="A93" s="19"/>
+      <c r="B93" s="19"/>
+      <c r="C93" s="20"/>
+      <c r="D93" s="20"/>
+      <c r="E93" s="19"/>
+      <c r="F93" s="18"/>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
@@ -5032,12 +4998,12 @@
       <c r="Z93" s="4"/>
     </row>
     <row r="94" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="20"/>
-      <c r="B94" s="20"/>
-      <c r="C94" s="19"/>
-      <c r="D94" s="19"/>
-      <c r="E94" s="20"/>
-      <c r="F94" s="17"/>
+      <c r="A94" s="19"/>
+      <c r="B94" s="19"/>
+      <c r="C94" s="18"/>
+      <c r="D94" s="18"/>
+      <c r="E94" s="19"/>
+      <c r="F94" s="16"/>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
       <c r="I94" s="4"/>
@@ -5060,12 +5026,12 @@
       <c r="Z94" s="4"/>
     </row>
     <row r="95" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A95" s="20"/>
-      <c r="B95" s="20"/>
-      <c r="C95" s="19"/>
-      <c r="D95" s="19"/>
-      <c r="E95" s="20"/>
-      <c r="F95" s="17"/>
+      <c r="A95" s="19"/>
+      <c r="B95" s="19"/>
+      <c r="C95" s="18"/>
+      <c r="D95" s="18"/>
+      <c r="E95" s="19"/>
+      <c r="F95" s="16"/>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
       <c r="I95" s="4"/>
@@ -5088,12 +5054,12 @@
       <c r="Z95" s="4"/>
     </row>
     <row r="96" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="20"/>
-      <c r="B96" s="20"/>
-      <c r="C96" s="19"/>
-      <c r="D96" s="19"/>
-      <c r="E96" s="20"/>
-      <c r="F96" s="17"/>
+      <c r="A96" s="19"/>
+      <c r="B96" s="19"/>
+      <c r="C96" s="18"/>
+      <c r="D96" s="18"/>
+      <c r="E96" s="19"/>
+      <c r="F96" s="16"/>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
       <c r="I96" s="4"/>
@@ -5116,12 +5082,12 @@
       <c r="Z96" s="4"/>
     </row>
     <row r="97" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="20"/>
-      <c r="B97" s="20"/>
-      <c r="C97" s="19"/>
-      <c r="D97" s="19"/>
-      <c r="E97" s="20"/>
-      <c r="F97" s="17"/>
+      <c r="A97" s="19"/>
+      <c r="B97" s="19"/>
+      <c r="C97" s="18"/>
+      <c r="D97" s="18"/>
+      <c r="E97" s="19"/>
+      <c r="F97" s="16"/>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
       <c r="I97" s="4"/>
@@ -5144,12 +5110,12 @@
       <c r="Z97" s="4"/>
     </row>
     <row r="98" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="20"/>
-      <c r="B98" s="20"/>
-      <c r="C98" s="19"/>
-      <c r="D98" s="19"/>
-      <c r="E98" s="20"/>
-      <c r="F98" s="17"/>
+      <c r="A98" s="19"/>
+      <c r="B98" s="19"/>
+      <c r="C98" s="18"/>
+      <c r="D98" s="18"/>
+      <c r="E98" s="19"/>
+      <c r="F98" s="16"/>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
       <c r="I98" s="4"/>
@@ -5172,12 +5138,12 @@
       <c r="Z98" s="4"/>
     </row>
     <row r="99" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="20"/>
-      <c r="B99" s="20"/>
-      <c r="C99" s="19"/>
-      <c r="D99" s="19"/>
-      <c r="E99" s="20"/>
-      <c r="F99" s="17"/>
+      <c r="A99" s="19"/>
+      <c r="B99" s="19"/>
+      <c r="C99" s="18"/>
+      <c r="D99" s="18"/>
+      <c r="E99" s="19"/>
+      <c r="F99" s="16"/>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
       <c r="I99" s="4"/>
@@ -5200,12 +5166,12 @@
       <c r="Z99" s="4"/>
     </row>
     <row r="100" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="20"/>
-      <c r="B100" s="20"/>
-      <c r="C100" s="19"/>
-      <c r="D100" s="19"/>
-      <c r="E100" s="20"/>
-      <c r="F100" s="17"/>
+      <c r="A100" s="19"/>
+      <c r="B100" s="19"/>
+      <c r="C100" s="18"/>
+      <c r="D100" s="18"/>
+      <c r="E100" s="19"/>
+      <c r="F100" s="16"/>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
       <c r="I100" s="4"/>
@@ -5228,12 +5194,12 @@
       <c r="Z100" s="4"/>
     </row>
     <row r="101" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A101" s="20"/>
-      <c r="B101" s="20"/>
-      <c r="C101" s="19"/>
-      <c r="D101" s="19"/>
-      <c r="E101" s="20"/>
-      <c r="F101" s="17"/>
+      <c r="A101" s="19"/>
+      <c r="B101" s="19"/>
+      <c r="C101" s="18"/>
+      <c r="D101" s="18"/>
+      <c r="E101" s="19"/>
+      <c r="F101" s="16"/>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
       <c r="I101" s="4"/>
@@ -5256,12 +5222,12 @@
       <c r="Z101" s="4"/>
     </row>
     <row r="102" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="20"/>
-      <c r="B102" s="20"/>
-      <c r="C102" s="19"/>
-      <c r="D102" s="19"/>
-      <c r="E102" s="20"/>
-      <c r="F102" s="17"/>
+      <c r="A102" s="19"/>
+      <c r="B102" s="19"/>
+      <c r="C102" s="18"/>
+      <c r="D102" s="18"/>
+      <c r="E102" s="19"/>
+      <c r="F102" s="16"/>
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
       <c r="I102" s="4"/>
@@ -5284,12 +5250,12 @@
       <c r="Z102" s="4"/>
     </row>
     <row r="103" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="20"/>
-      <c r="B103" s="20"/>
-      <c r="C103" s="19"/>
-      <c r="D103" s="19"/>
-      <c r="E103" s="20"/>
-      <c r="F103" s="17"/>
+      <c r="A103" s="19"/>
+      <c r="B103" s="19"/>
+      <c r="C103" s="18"/>
+      <c r="D103" s="18"/>
+      <c r="E103" s="19"/>
+      <c r="F103" s="16"/>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
       <c r="I103" s="4"/>
@@ -5312,12 +5278,12 @@
       <c r="Z103" s="4"/>
     </row>
     <row r="104" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A104" s="20"/>
-      <c r="B104" s="20"/>
-      <c r="C104" s="19"/>
-      <c r="D104" s="19"/>
-      <c r="E104" s="20"/>
-      <c r="F104" s="17"/>
+      <c r="A104" s="19"/>
+      <c r="B104" s="19"/>
+      <c r="C104" s="18"/>
+      <c r="D104" s="18"/>
+      <c r="E104" s="19"/>
+      <c r="F104" s="16"/>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
       <c r="I104" s="4"/>
@@ -5340,12 +5306,12 @@
       <c r="Z104" s="4"/>
     </row>
     <row r="105" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A105" s="20"/>
-      <c r="B105" s="20"/>
-      <c r="C105" s="19"/>
-      <c r="D105" s="19"/>
-      <c r="E105" s="20"/>
-      <c r="F105" s="17"/>
+      <c r="A105" s="19"/>
+      <c r="B105" s="19"/>
+      <c r="C105" s="18"/>
+      <c r="D105" s="18"/>
+      <c r="E105" s="19"/>
+      <c r="F105" s="16"/>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
       <c r="I105" s="4"/>
@@ -5368,12 +5334,12 @@
       <c r="Z105" s="4"/>
     </row>
     <row r="106" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="20"/>
-      <c r="B106" s="20"/>
-      <c r="C106" s="21"/>
-      <c r="D106" s="21"/>
-      <c r="E106" s="20"/>
-      <c r="F106" s="19"/>
+      <c r="A106" s="19"/>
+      <c r="B106" s="19"/>
+      <c r="C106" s="20"/>
+      <c r="D106" s="20"/>
+      <c r="E106" s="19"/>
+      <c r="F106" s="18"/>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
       <c r="I106" s="4"/>
@@ -5396,12 +5362,12 @@
       <c r="Z106" s="4"/>
     </row>
     <row r="107" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A107" s="20"/>
-      <c r="B107" s="20"/>
-      <c r="C107" s="19"/>
-      <c r="D107" s="19"/>
-      <c r="E107" s="20"/>
-      <c r="F107" s="17"/>
+      <c r="A107" s="19"/>
+      <c r="B107" s="19"/>
+      <c r="C107" s="18"/>
+      <c r="D107" s="18"/>
+      <c r="E107" s="19"/>
+      <c r="F107" s="16"/>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
       <c r="I107" s="4"/>
@@ -5424,12 +5390,12 @@
       <c r="Z107" s="4"/>
     </row>
     <row r="108" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="20"/>
-      <c r="B108" s="20"/>
-      <c r="C108" s="19"/>
-      <c r="D108" s="19"/>
-      <c r="E108" s="20"/>
-      <c r="F108" s="17"/>
+      <c r="A108" s="19"/>
+      <c r="B108" s="19"/>
+      <c r="C108" s="18"/>
+      <c r="D108" s="18"/>
+      <c r="E108" s="19"/>
+      <c r="F108" s="16"/>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
       <c r="I108" s="4"/>
@@ -5452,12 +5418,12 @@
       <c r="Z108" s="4"/>
     </row>
     <row r="109" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A109" s="20"/>
-      <c r="B109" s="20"/>
-      <c r="C109" s="19"/>
-      <c r="D109" s="19"/>
-      <c r="E109" s="20"/>
-      <c r="F109" s="17"/>
+      <c r="A109" s="19"/>
+      <c r="B109" s="19"/>
+      <c r="C109" s="18"/>
+      <c r="D109" s="18"/>
+      <c r="E109" s="19"/>
+      <c r="F109" s="16"/>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
       <c r="I109" s="4"/>
@@ -5480,12 +5446,12 @@
       <c r="Z109" s="4"/>
     </row>
     <row r="110" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A110" s="20"/>
-      <c r="B110" s="20"/>
-      <c r="C110" s="19"/>
-      <c r="D110" s="19"/>
-      <c r="E110" s="20"/>
-      <c r="F110" s="17"/>
+      <c r="A110" s="19"/>
+      <c r="B110" s="19"/>
+      <c r="C110" s="18"/>
+      <c r="D110" s="18"/>
+      <c r="E110" s="19"/>
+      <c r="F110" s="16"/>
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
       <c r="I110" s="4"/>
@@ -5508,12 +5474,12 @@
       <c r="Z110" s="4"/>
     </row>
     <row r="111" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A111" s="20"/>
-      <c r="B111" s="20"/>
-      <c r="C111" s="19"/>
-      <c r="D111" s="19"/>
-      <c r="E111" s="20"/>
-      <c r="F111" s="17"/>
+      <c r="A111" s="19"/>
+      <c r="B111" s="19"/>
+      <c r="C111" s="18"/>
+      <c r="D111" s="18"/>
+      <c r="E111" s="19"/>
+      <c r="F111" s="16"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
       <c r="I111" s="4"/>
@@ -5536,12 +5502,12 @@
       <c r="Z111" s="4"/>
     </row>
     <row r="112" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A112" s="20"/>
-      <c r="B112" s="20"/>
-      <c r="C112" s="19"/>
-      <c r="D112" s="19"/>
-      <c r="E112" s="20"/>
-      <c r="F112" s="17"/>
+      <c r="A112" s="19"/>
+      <c r="B112" s="19"/>
+      <c r="C112" s="18"/>
+      <c r="D112" s="18"/>
+      <c r="E112" s="19"/>
+      <c r="F112" s="16"/>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
       <c r="I112" s="4"/>
@@ -5564,12 +5530,12 @@
       <c r="Z112" s="4"/>
     </row>
     <row r="113" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A113" s="20"/>
-      <c r="B113" s="20"/>
-      <c r="C113" s="19"/>
-      <c r="D113" s="19"/>
-      <c r="E113" s="20"/>
-      <c r="F113" s="17"/>
+      <c r="A113" s="19"/>
+      <c r="B113" s="19"/>
+      <c r="C113" s="18"/>
+      <c r="D113" s="18"/>
+      <c r="E113" s="19"/>
+      <c r="F113" s="16"/>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
       <c r="I113" s="4"/>
@@ -5592,12 +5558,12 @@
       <c r="Z113" s="4"/>
     </row>
     <row r="114" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A114" s="20"/>
-      <c r="B114" s="20"/>
-      <c r="C114" s="19"/>
-      <c r="D114" s="19"/>
-      <c r="E114" s="20"/>
-      <c r="F114" s="17"/>
+      <c r="A114" s="19"/>
+      <c r="B114" s="19"/>
+      <c r="C114" s="18"/>
+      <c r="D114" s="18"/>
+      <c r="E114" s="19"/>
+      <c r="F114" s="16"/>
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
       <c r="I114" s="4"/>
@@ -5620,12 +5586,12 @@
       <c r="Z114" s="4"/>
     </row>
     <row r="115" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A115" s="20"/>
-      <c r="B115" s="20"/>
-      <c r="C115" s="19"/>
-      <c r="D115" s="19"/>
-      <c r="E115" s="20"/>
-      <c r="F115" s="17"/>
+      <c r="A115" s="19"/>
+      <c r="B115" s="19"/>
+      <c r="C115" s="18"/>
+      <c r="D115" s="18"/>
+      <c r="E115" s="19"/>
+      <c r="F115" s="16"/>
       <c r="G115" s="4"/>
       <c r="H115" s="4"/>
       <c r="I115" s="4"/>
@@ -5648,12 +5614,12 @@
       <c r="Z115" s="4"/>
     </row>
     <row r="116" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A116" s="20"/>
-      <c r="B116" s="20"/>
-      <c r="C116" s="21"/>
-      <c r="D116" s="21"/>
-      <c r="E116" s="20"/>
-      <c r="F116" s="19"/>
+      <c r="A116" s="19"/>
+      <c r="B116" s="19"/>
+      <c r="C116" s="20"/>
+      <c r="D116" s="20"/>
+      <c r="E116" s="19"/>
+      <c r="F116" s="18"/>
       <c r="G116" s="4"/>
       <c r="H116" s="4"/>
       <c r="I116" s="4"/>
@@ -5676,12 +5642,12 @@
       <c r="Z116" s="4"/>
     </row>
     <row r="117" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A117" s="20"/>
-      <c r="B117" s="20"/>
-      <c r="C117" s="21"/>
-      <c r="D117" s="21"/>
-      <c r="E117" s="20"/>
-      <c r="F117" s="19"/>
+      <c r="A117" s="19"/>
+      <c r="B117" s="19"/>
+      <c r="C117" s="20"/>
+      <c r="D117" s="20"/>
+      <c r="E117" s="19"/>
+      <c r="F117" s="18"/>
       <c r="G117" s="4"/>
       <c r="H117" s="4"/>
       <c r="I117" s="4"/>
@@ -5704,12 +5670,12 @@
       <c r="Z117" s="4"/>
     </row>
     <row r="118" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="20"/>
-      <c r="B118" s="20"/>
-      <c r="C118" s="21"/>
-      <c r="D118" s="21"/>
-      <c r="E118" s="20"/>
-      <c r="F118" s="19"/>
+      <c r="A118" s="19"/>
+      <c r="B118" s="19"/>
+      <c r="C118" s="20"/>
+      <c r="D118" s="20"/>
+      <c r="E118" s="19"/>
+      <c r="F118" s="18"/>
       <c r="G118" s="4"/>
       <c r="H118" s="4"/>
       <c r="I118" s="4"/>
@@ -5732,12 +5698,12 @@
       <c r="Z118" s="4"/>
     </row>
     <row r="119" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A119" s="20"/>
-      <c r="B119" s="20"/>
-      <c r="C119" s="21"/>
-      <c r="D119" s="21"/>
-      <c r="E119" s="20"/>
-      <c r="F119" s="19"/>
+      <c r="A119" s="19"/>
+      <c r="B119" s="19"/>
+      <c r="C119" s="20"/>
+      <c r="D119" s="20"/>
+      <c r="E119" s="19"/>
+      <c r="F119" s="18"/>
       <c r="G119" s="4"/>
       <c r="H119" s="4"/>
       <c r="I119" s="4"/>
@@ -5760,12 +5726,12 @@
       <c r="Z119" s="4"/>
     </row>
     <row r="120" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A120" s="20"/>
-      <c r="B120" s="20"/>
-      <c r="C120" s="21"/>
-      <c r="D120" s="21"/>
-      <c r="E120" s="20"/>
-      <c r="F120" s="19"/>
+      <c r="A120" s="19"/>
+      <c r="B120" s="19"/>
+      <c r="C120" s="20"/>
+      <c r="D120" s="20"/>
+      <c r="E120" s="19"/>
+      <c r="F120" s="18"/>
       <c r="G120" s="4"/>
       <c r="H120" s="4"/>
       <c r="I120" s="4"/>
@@ -5788,12 +5754,12 @@
       <c r="Z120" s="4"/>
     </row>
     <row r="121" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A121" s="20"/>
-      <c r="B121" s="20"/>
-      <c r="C121" s="21"/>
-      <c r="D121" s="21"/>
-      <c r="E121" s="20"/>
-      <c r="F121" s="19"/>
+      <c r="A121" s="19"/>
+      <c r="B121" s="19"/>
+      <c r="C121" s="20"/>
+      <c r="D121" s="20"/>
+      <c r="E121" s="19"/>
+      <c r="F121" s="18"/>
       <c r="G121" s="4"/>
       <c r="H121" s="4"/>
       <c r="I121" s="4"/>
@@ -5816,12 +5782,12 @@
       <c r="Z121" s="4"/>
     </row>
     <row r="122" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A122" s="20"/>
-      <c r="B122" s="20"/>
-      <c r="C122" s="19"/>
-      <c r="D122" s="19"/>
-      <c r="E122" s="20"/>
-      <c r="F122" s="17"/>
+      <c r="A122" s="19"/>
+      <c r="B122" s="19"/>
+      <c r="C122" s="18"/>
+      <c r="D122" s="18"/>
+      <c r="E122" s="19"/>
+      <c r="F122" s="16"/>
       <c r="G122" s="4"/>
       <c r="H122" s="4"/>
       <c r="I122" s="4"/>
@@ -5844,12 +5810,12 @@
       <c r="Z122" s="4"/>
     </row>
     <row r="123" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A123" s="20"/>
-      <c r="B123" s="20"/>
-      <c r="C123" s="21"/>
-      <c r="D123" s="21"/>
-      <c r="E123" s="20"/>
-      <c r="F123" s="19"/>
+      <c r="A123" s="19"/>
+      <c r="B123" s="19"/>
+      <c r="C123" s="20"/>
+      <c r="D123" s="20"/>
+      <c r="E123" s="19"/>
+      <c r="F123" s="18"/>
       <c r="G123" s="4"/>
       <c r="H123" s="4"/>
       <c r="I123" s="4"/>
@@ -5872,12 +5838,12 @@
       <c r="Z123" s="4"/>
     </row>
     <row r="124" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A124" s="20"/>
-      <c r="B124" s="20"/>
-      <c r="C124" s="21"/>
-      <c r="D124" s="21"/>
-      <c r="E124" s="20"/>
-      <c r="F124" s="19"/>
+      <c r="A124" s="19"/>
+      <c r="B124" s="19"/>
+      <c r="C124" s="20"/>
+      <c r="D124" s="20"/>
+      <c r="E124" s="19"/>
+      <c r="F124" s="18"/>
       <c r="G124" s="4"/>
       <c r="H124" s="4"/>
       <c r="I124" s="4"/>
@@ -5900,12 +5866,12 @@
       <c r="Z124" s="4"/>
     </row>
     <row r="125" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A125" s="20"/>
-      <c r="B125" s="20"/>
-      <c r="C125" s="19"/>
-      <c r="D125" s="19"/>
-      <c r="E125" s="20"/>
-      <c r="F125" s="17"/>
+      <c r="A125" s="19"/>
+      <c r="B125" s="19"/>
+      <c r="C125" s="18"/>
+      <c r="D125" s="18"/>
+      <c r="E125" s="19"/>
+      <c r="F125" s="16"/>
       <c r="G125" s="4"/>
       <c r="H125" s="4"/>
       <c r="I125" s="4"/>
@@ -5928,12 +5894,12 @@
       <c r="Z125" s="4"/>
     </row>
     <row r="126" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A126" s="20"/>
-      <c r="B126" s="20"/>
-      <c r="C126" s="21"/>
-      <c r="D126" s="21"/>
-      <c r="E126" s="20"/>
-      <c r="F126" s="19"/>
+      <c r="A126" s="19"/>
+      <c r="B126" s="19"/>
+      <c r="C126" s="20"/>
+      <c r="D126" s="20"/>
+      <c r="E126" s="19"/>
+      <c r="F126" s="18"/>
       <c r="G126" s="4"/>
       <c r="H126" s="4"/>
       <c r="I126" s="4"/>
@@ -5956,12 +5922,12 @@
       <c r="Z126" s="4"/>
     </row>
     <row r="127" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A127" s="20"/>
-      <c r="B127" s="20"/>
-      <c r="C127" s="21"/>
-      <c r="D127" s="21"/>
-      <c r="E127" s="20"/>
-      <c r="F127" s="19"/>
+      <c r="A127" s="19"/>
+      <c r="B127" s="19"/>
+      <c r="C127" s="20"/>
+      <c r="D127" s="20"/>
+      <c r="E127" s="19"/>
+      <c r="F127" s="18"/>
       <c r="G127" s="4"/>
       <c r="H127" s="4"/>
       <c r="I127" s="4"/>
@@ -5984,12 +5950,12 @@
       <c r="Z127" s="4"/>
     </row>
     <row r="128" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A128" s="20"/>
-      <c r="B128" s="20"/>
-      <c r="C128" s="21"/>
-      <c r="D128" s="21"/>
-      <c r="E128" s="20"/>
-      <c r="F128" s="19"/>
+      <c r="A128" s="19"/>
+      <c r="B128" s="19"/>
+      <c r="C128" s="20"/>
+      <c r="D128" s="20"/>
+      <c r="E128" s="19"/>
+      <c r="F128" s="18"/>
       <c r="G128" s="4"/>
       <c r="H128" s="4"/>
       <c r="I128" s="4"/>
@@ -6012,12 +5978,12 @@
       <c r="Z128" s="4"/>
     </row>
     <row r="129" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A129" s="20"/>
-      <c r="B129" s="20"/>
-      <c r="C129" s="19"/>
-      <c r="D129" s="19"/>
-      <c r="E129" s="20"/>
-      <c r="F129" s="17"/>
+      <c r="A129" s="19"/>
+      <c r="B129" s="19"/>
+      <c r="C129" s="18"/>
+      <c r="D129" s="18"/>
+      <c r="E129" s="19"/>
+      <c r="F129" s="16"/>
       <c r="G129" s="4"/>
       <c r="H129" s="4"/>
       <c r="I129" s="4"/>
@@ -6040,12 +6006,12 @@
       <c r="Z129" s="4"/>
     </row>
     <row r="130" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A130" s="20"/>
-      <c r="B130" s="20"/>
-      <c r="C130" s="19"/>
-      <c r="D130" s="19"/>
-      <c r="E130" s="20"/>
-      <c r="F130" s="17"/>
+      <c r="A130" s="19"/>
+      <c r="B130" s="19"/>
+      <c r="C130" s="18"/>
+      <c r="D130" s="18"/>
+      <c r="E130" s="19"/>
+      <c r="F130" s="16"/>
       <c r="G130" s="4"/>
       <c r="H130" s="4"/>
       <c r="I130" s="4"/>
@@ -6068,12 +6034,12 @@
       <c r="Z130" s="4"/>
     </row>
     <row r="131" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A131" s="20"/>
-      <c r="B131" s="20"/>
-      <c r="C131" s="19"/>
-      <c r="D131" s="19"/>
-      <c r="E131" s="20"/>
-      <c r="F131" s="17"/>
+      <c r="A131" s="19"/>
+      <c r="B131" s="19"/>
+      <c r="C131" s="18"/>
+      <c r="D131" s="18"/>
+      <c r="E131" s="19"/>
+      <c r="F131" s="16"/>
       <c r="G131" s="4"/>
       <c r="H131" s="4"/>
       <c r="I131" s="4"/>
@@ -6096,12 +6062,12 @@
       <c r="Z131" s="4"/>
     </row>
     <row r="132" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A132" s="20"/>
-      <c r="B132" s="20"/>
-      <c r="C132" s="19"/>
-      <c r="D132" s="19"/>
-      <c r="E132" s="20"/>
-      <c r="F132" s="17"/>
+      <c r="A132" s="19"/>
+      <c r="B132" s="19"/>
+      <c r="C132" s="18"/>
+      <c r="D132" s="18"/>
+      <c r="E132" s="19"/>
+      <c r="F132" s="16"/>
       <c r="G132" s="4"/>
       <c r="H132" s="4"/>
       <c r="I132" s="4"/>
@@ -6124,12 +6090,12 @@
       <c r="Z132" s="4"/>
     </row>
     <row r="133" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A133" s="20"/>
-      <c r="B133" s="20"/>
-      <c r="C133" s="19"/>
-      <c r="D133" s="19"/>
-      <c r="E133" s="20"/>
-      <c r="F133" s="17"/>
+      <c r="A133" s="19"/>
+      <c r="B133" s="19"/>
+      <c r="C133" s="18"/>
+      <c r="D133" s="18"/>
+      <c r="E133" s="19"/>
+      <c r="F133" s="16"/>
       <c r="G133" s="4"/>
       <c r="H133" s="4"/>
       <c r="I133" s="4"/>
@@ -6152,12 +6118,12 @@
       <c r="Z133" s="4"/>
     </row>
     <row r="134" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A134" s="20"/>
-      <c r="B134" s="20"/>
-      <c r="C134" s="21"/>
-      <c r="D134" s="21"/>
-      <c r="E134" s="20"/>
-      <c r="F134" s="19"/>
+      <c r="A134" s="19"/>
+      <c r="B134" s="19"/>
+      <c r="C134" s="20"/>
+      <c r="D134" s="20"/>
+      <c r="E134" s="19"/>
+      <c r="F134" s="18"/>
       <c r="G134" s="4"/>
       <c r="H134" s="4"/>
       <c r="I134" s="4"/>
@@ -6180,12 +6146,12 @@
       <c r="Z134" s="4"/>
     </row>
     <row r="135" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A135" s="20"/>
-      <c r="B135" s="20"/>
-      <c r="C135" s="19"/>
-      <c r="D135" s="19"/>
-      <c r="E135" s="20"/>
-      <c r="F135" s="17"/>
+      <c r="A135" s="19"/>
+      <c r="B135" s="19"/>
+      <c r="C135" s="18"/>
+      <c r="D135" s="18"/>
+      <c r="E135" s="19"/>
+      <c r="F135" s="16"/>
       <c r="G135" s="4"/>
       <c r="H135" s="4"/>
       <c r="I135" s="4"/>
@@ -6208,12 +6174,12 @@
       <c r="Z135" s="4"/>
     </row>
     <row r="136" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A136" s="20"/>
-      <c r="B136" s="20"/>
-      <c r="C136" s="19"/>
-      <c r="D136" s="19"/>
-      <c r="E136" s="20"/>
-      <c r="F136" s="17"/>
+      <c r="A136" s="19"/>
+      <c r="B136" s="19"/>
+      <c r="C136" s="18"/>
+      <c r="D136" s="18"/>
+      <c r="E136" s="19"/>
+      <c r="F136" s="16"/>
       <c r="G136" s="4"/>
       <c r="H136" s="4"/>
       <c r="I136" s="4"/>
@@ -6236,12 +6202,12 @@
       <c r="Z136" s="4"/>
     </row>
     <row r="137" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A137" s="20"/>
-      <c r="B137" s="20"/>
-      <c r="C137" s="19"/>
-      <c r="D137" s="19"/>
-      <c r="E137" s="20"/>
-      <c r="F137" s="17"/>
+      <c r="A137" s="19"/>
+      <c r="B137" s="19"/>
+      <c r="C137" s="18"/>
+      <c r="D137" s="18"/>
+      <c r="E137" s="19"/>
+      <c r="F137" s="16"/>
       <c r="G137" s="4"/>
       <c r="H137" s="4"/>
       <c r="I137" s="4"/>
@@ -6264,12 +6230,12 @@
       <c r="Z137" s="4"/>
     </row>
     <row r="138" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A138" s="20"/>
-      <c r="B138" s="20"/>
-      <c r="C138" s="19"/>
-      <c r="D138" s="19"/>
-      <c r="E138" s="20"/>
-      <c r="F138" s="17"/>
+      <c r="A138" s="19"/>
+      <c r="B138" s="19"/>
+      <c r="C138" s="18"/>
+      <c r="D138" s="18"/>
+      <c r="E138" s="19"/>
+      <c r="F138" s="16"/>
       <c r="G138" s="4"/>
       <c r="H138" s="4"/>
       <c r="I138" s="4"/>
@@ -6292,12 +6258,12 @@
       <c r="Z138" s="4"/>
     </row>
     <row r="139" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A139" s="20"/>
-      <c r="B139" s="20"/>
-      <c r="C139" s="21"/>
-      <c r="D139" s="21"/>
-      <c r="E139" s="20"/>
-      <c r="F139" s="19"/>
+      <c r="A139" s="19"/>
+      <c r="B139" s="19"/>
+      <c r="C139" s="20"/>
+      <c r="D139" s="20"/>
+      <c r="E139" s="19"/>
+      <c r="F139" s="18"/>
       <c r="G139" s="4"/>
       <c r="H139" s="4"/>
       <c r="I139" s="4"/>
@@ -6320,12 +6286,12 @@
       <c r="Z139" s="4"/>
     </row>
     <row r="140" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A140" s="20"/>
-      <c r="B140" s="20"/>
-      <c r="C140" s="21"/>
-      <c r="D140" s="21"/>
-      <c r="E140" s="20"/>
-      <c r="F140" s="19"/>
+      <c r="A140" s="19"/>
+      <c r="B140" s="19"/>
+      <c r="C140" s="20"/>
+      <c r="D140" s="20"/>
+      <c r="E140" s="19"/>
+      <c r="F140" s="18"/>
       <c r="G140" s="4"/>
       <c r="H140" s="4"/>
       <c r="I140" s="4"/>
@@ -6348,12 +6314,12 @@
       <c r="Z140" s="4"/>
     </row>
     <row r="141" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A141" s="20"/>
-      <c r="B141" s="20"/>
-      <c r="C141" s="21"/>
-      <c r="D141" s="21"/>
-      <c r="E141" s="20"/>
-      <c r="F141" s="19"/>
+      <c r="A141" s="19"/>
+      <c r="B141" s="19"/>
+      <c r="C141" s="20"/>
+      <c r="D141" s="20"/>
+      <c r="E141" s="19"/>
+      <c r="F141" s="18"/>
       <c r="G141" s="4"/>
       <c r="H141" s="4"/>
       <c r="I141" s="4"/>
@@ -6376,12 +6342,12 @@
       <c r="Z141" s="4"/>
     </row>
     <row r="142" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A142" s="20"/>
-      <c r="B142" s="20"/>
-      <c r="C142" s="19"/>
-      <c r="D142" s="19"/>
-      <c r="E142" s="20"/>
-      <c r="F142" s="17"/>
+      <c r="A142" s="19"/>
+      <c r="B142" s="19"/>
+      <c r="C142" s="18"/>
+      <c r="D142" s="18"/>
+      <c r="E142" s="19"/>
+      <c r="F142" s="16"/>
       <c r="G142" s="4"/>
       <c r="H142" s="4"/>
       <c r="I142" s="4"/>
@@ -6404,12 +6370,12 @@
       <c r="Z142" s="4"/>
     </row>
     <row r="143" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A143" s="20"/>
-      <c r="B143" s="20"/>
-      <c r="C143" s="21"/>
-      <c r="D143" s="21"/>
-      <c r="E143" s="20"/>
-      <c r="F143" s="19"/>
+      <c r="A143" s="19"/>
+      <c r="B143" s="19"/>
+      <c r="C143" s="20"/>
+      <c r="D143" s="20"/>
+      <c r="E143" s="19"/>
+      <c r="F143" s="18"/>
       <c r="G143" s="4"/>
       <c r="H143" s="4"/>
       <c r="I143" s="4"/>
@@ -6432,12 +6398,12 @@
       <c r="Z143" s="4"/>
     </row>
     <row r="144" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A144" s="20"/>
-      <c r="B144" s="20"/>
-      <c r="C144" s="19"/>
-      <c r="D144" s="19"/>
-      <c r="E144" s="20"/>
-      <c r="F144" s="17"/>
+      <c r="A144" s="19"/>
+      <c r="B144" s="19"/>
+      <c r="C144" s="18"/>
+      <c r="D144" s="18"/>
+      <c r="E144" s="19"/>
+      <c r="F144" s="16"/>
       <c r="G144" s="4"/>
       <c r="H144" s="4"/>
       <c r="I144" s="4"/>
@@ -6460,12 +6426,12 @@
       <c r="Z144" s="4"/>
     </row>
     <row r="145" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A145" s="20"/>
-      <c r="B145" s="20"/>
-      <c r="C145" s="21"/>
-      <c r="D145" s="21"/>
-      <c r="E145" s="20"/>
-      <c r="F145" s="19"/>
+      <c r="A145" s="19"/>
+      <c r="B145" s="19"/>
+      <c r="C145" s="20"/>
+      <c r="D145" s="20"/>
+      <c r="E145" s="19"/>
+      <c r="F145" s="18"/>
       <c r="G145" s="4"/>
       <c r="H145" s="4"/>
       <c r="I145" s="4"/>
@@ -6488,12 +6454,12 @@
       <c r="Z145" s="4"/>
     </row>
     <row r="146" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A146" s="20"/>
-      <c r="B146" s="20"/>
-      <c r="C146" s="19"/>
-      <c r="D146" s="19"/>
-      <c r="E146" s="20"/>
-      <c r="F146" s="17"/>
+      <c r="A146" s="19"/>
+      <c r="B146" s="19"/>
+      <c r="C146" s="18"/>
+      <c r="D146" s="18"/>
+      <c r="E146" s="19"/>
+      <c r="F146" s="16"/>
       <c r="G146" s="4"/>
       <c r="H146" s="4"/>
       <c r="I146" s="4"/>
@@ -6516,12 +6482,12 @@
       <c r="Z146" s="4"/>
     </row>
     <row r="147" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A147" s="20"/>
-      <c r="B147" s="20"/>
-      <c r="C147" s="21"/>
-      <c r="D147" s="21"/>
-      <c r="E147" s="20"/>
-      <c r="F147" s="19"/>
+      <c r="A147" s="19"/>
+      <c r="B147" s="19"/>
+      <c r="C147" s="20"/>
+      <c r="D147" s="20"/>
+      <c r="E147" s="19"/>
+      <c r="F147" s="18"/>
       <c r="G147" s="4"/>
       <c r="H147" s="4"/>
       <c r="I147" s="4"/>
@@ -6544,12 +6510,12 @@
       <c r="Z147" s="4"/>
     </row>
     <row r="148" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A148" s="20"/>
-      <c r="B148" s="20"/>
-      <c r="C148" s="21"/>
-      <c r="D148" s="21"/>
-      <c r="E148" s="20"/>
-      <c r="F148" s="19"/>
+      <c r="A148" s="19"/>
+      <c r="B148" s="19"/>
+      <c r="C148" s="20"/>
+      <c r="D148" s="20"/>
+      <c r="E148" s="19"/>
+      <c r="F148" s="18"/>
       <c r="G148" s="4"/>
       <c r="H148" s="4"/>
       <c r="I148" s="4"/>
@@ -6572,12 +6538,12 @@
       <c r="Z148" s="4"/>
     </row>
     <row r="149" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="20"/>
-      <c r="B149" s="20"/>
-      <c r="C149" s="21"/>
-      <c r="D149" s="21"/>
-      <c r="E149" s="20"/>
-      <c r="F149" s="19"/>
+      <c r="A149" s="19"/>
+      <c r="B149" s="19"/>
+      <c r="C149" s="20"/>
+      <c r="D149" s="20"/>
+      <c r="E149" s="19"/>
+      <c r="F149" s="18"/>
       <c r="G149" s="4"/>
       <c r="H149" s="4"/>
       <c r="I149" s="4"/>
@@ -6600,12 +6566,12 @@
       <c r="Z149" s="4"/>
     </row>
     <row r="150" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A150" s="20"/>
-      <c r="B150" s="20"/>
-      <c r="C150" s="21"/>
-      <c r="D150" s="21"/>
-      <c r="E150" s="20"/>
-      <c r="F150" s="19"/>
+      <c r="A150" s="19"/>
+      <c r="B150" s="19"/>
+      <c r="C150" s="20"/>
+      <c r="D150" s="20"/>
+      <c r="E150" s="19"/>
+      <c r="F150" s="18"/>
       <c r="G150" s="4"/>
       <c r="H150" s="4"/>
       <c r="I150" s="4"/>
@@ -6628,12 +6594,12 @@
       <c r="Z150" s="4"/>
     </row>
     <row r="151" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A151" s="20"/>
-      <c r="B151" s="20"/>
-      <c r="C151" s="19"/>
-      <c r="D151" s="19"/>
-      <c r="E151" s="20"/>
-      <c r="F151" s="17"/>
+      <c r="A151" s="19"/>
+      <c r="B151" s="19"/>
+      <c r="C151" s="18"/>
+      <c r="D151" s="18"/>
+      <c r="E151" s="19"/>
+      <c r="F151" s="16"/>
       <c r="G151" s="4"/>
       <c r="H151" s="4"/>
       <c r="I151" s="4"/>
@@ -6656,12 +6622,12 @@
       <c r="Z151" s="4"/>
     </row>
     <row r="152" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A152" s="20"/>
-      <c r="B152" s="20"/>
-      <c r="C152" s="21"/>
-      <c r="D152" s="21"/>
-      <c r="E152" s="20"/>
-      <c r="F152" s="19"/>
+      <c r="A152" s="19"/>
+      <c r="B152" s="19"/>
+      <c r="C152" s="20"/>
+      <c r="D152" s="20"/>
+      <c r="E152" s="19"/>
+      <c r="F152" s="18"/>
       <c r="G152" s="4"/>
       <c r="H152" s="4"/>
       <c r="I152" s="4"/>
@@ -6684,12 +6650,12 @@
       <c r="Z152" s="4"/>
     </row>
     <row r="153" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A153" s="20"/>
-      <c r="B153" s="20"/>
-      <c r="C153" s="19"/>
-      <c r="D153" s="19"/>
-      <c r="E153" s="20"/>
-      <c r="F153" s="17"/>
+      <c r="A153" s="19"/>
+      <c r="B153" s="19"/>
+      <c r="C153" s="18"/>
+      <c r="D153" s="18"/>
+      <c r="E153" s="19"/>
+      <c r="F153" s="16"/>
       <c r="G153" s="4"/>
       <c r="H153" s="4"/>
       <c r="I153" s="4"/>
@@ -6712,12 +6678,12 @@
       <c r="Z153" s="4"/>
     </row>
     <row r="154" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A154" s="20"/>
-      <c r="B154" s="20"/>
-      <c r="C154" s="19"/>
-      <c r="D154" s="19"/>
-      <c r="E154" s="20"/>
-      <c r="F154" s="17"/>
+      <c r="A154" s="19"/>
+      <c r="B154" s="19"/>
+      <c r="C154" s="18"/>
+      <c r="D154" s="18"/>
+      <c r="E154" s="19"/>
+      <c r="F154" s="16"/>
       <c r="G154" s="4"/>
       <c r="H154" s="4"/>
       <c r="I154" s="4"/>
@@ -6740,12 +6706,12 @@
       <c r="Z154" s="4"/>
     </row>
     <row r="155" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A155" s="20"/>
-      <c r="B155" s="20"/>
-      <c r="C155" s="21"/>
-      <c r="D155" s="21"/>
-      <c r="E155" s="20"/>
-      <c r="F155" s="19"/>
+      <c r="A155" s="19"/>
+      <c r="B155" s="19"/>
+      <c r="C155" s="20"/>
+      <c r="D155" s="20"/>
+      <c r="E155" s="19"/>
+      <c r="F155" s="18"/>
       <c r="G155" s="4"/>
       <c r="H155" s="4"/>
       <c r="I155" s="4"/>
@@ -6768,12 +6734,12 @@
       <c r="Z155" s="4"/>
     </row>
     <row r="156" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A156" s="20"/>
-      <c r="B156" s="20"/>
-      <c r="C156" s="21"/>
-      <c r="D156" s="21"/>
-      <c r="E156" s="20"/>
-      <c r="F156" s="19"/>
+      <c r="A156" s="19"/>
+      <c r="B156" s="19"/>
+      <c r="C156" s="20"/>
+      <c r="D156" s="20"/>
+      <c r="E156" s="19"/>
+      <c r="F156" s="18"/>
       <c r="G156" s="4"/>
       <c r="H156" s="4"/>
       <c r="I156" s="4"/>
@@ -6796,12 +6762,12 @@
       <c r="Z156" s="4"/>
     </row>
     <row r="157" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A157" s="20"/>
-      <c r="B157" s="20"/>
-      <c r="C157" s="21"/>
-      <c r="D157" s="21"/>
-      <c r="E157" s="20"/>
-      <c r="F157" s="19"/>
+      <c r="A157" s="19"/>
+      <c r="B157" s="19"/>
+      <c r="C157" s="20"/>
+      <c r="D157" s="20"/>
+      <c r="E157" s="19"/>
+      <c r="F157" s="18"/>
       <c r="G157" s="4"/>
       <c r="H157" s="4"/>
       <c r="I157" s="4"/>
@@ -6824,12 +6790,12 @@
       <c r="Z157" s="4"/>
     </row>
     <row r="158" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A158" s="20"/>
-      <c r="B158" s="20"/>
-      <c r="C158" s="21"/>
-      <c r="D158" s="21"/>
-      <c r="E158" s="20"/>
-      <c r="F158" s="19"/>
+      <c r="A158" s="19"/>
+      <c r="B158" s="19"/>
+      <c r="C158" s="20"/>
+      <c r="D158" s="20"/>
+      <c r="E158" s="19"/>
+      <c r="F158" s="18"/>
       <c r="G158" s="4"/>
       <c r="H158" s="4"/>
       <c r="I158" s="4"/>
@@ -6852,12 +6818,12 @@
       <c r="Z158" s="4"/>
     </row>
     <row r="159" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A159" s="20"/>
-      <c r="B159" s="20"/>
-      <c r="C159" s="21"/>
-      <c r="D159" s="21"/>
-      <c r="E159" s="20"/>
-      <c r="F159" s="19"/>
+      <c r="A159" s="19"/>
+      <c r="B159" s="19"/>
+      <c r="C159" s="20"/>
+      <c r="D159" s="20"/>
+      <c r="E159" s="19"/>
+      <c r="F159" s="18"/>
       <c r="G159" s="4"/>
       <c r="H159" s="4"/>
       <c r="I159" s="4"/>
@@ -6880,12 +6846,12 @@
       <c r="Z159" s="4"/>
     </row>
     <row r="160" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A160" s="20"/>
-      <c r="B160" s="20"/>
-      <c r="C160" s="21"/>
-      <c r="D160" s="21"/>
-      <c r="E160" s="20"/>
-      <c r="F160" s="19"/>
+      <c r="A160" s="19"/>
+      <c r="B160" s="19"/>
+      <c r="C160" s="20"/>
+      <c r="D160" s="20"/>
+      <c r="E160" s="19"/>
+      <c r="F160" s="18"/>
       <c r="G160" s="4"/>
       <c r="H160" s="4"/>
       <c r="I160" s="4"/>
@@ -6908,12 +6874,12 @@
       <c r="Z160" s="4"/>
     </row>
     <row r="161" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A161" s="20"/>
-      <c r="B161" s="20"/>
-      <c r="C161" s="21"/>
-      <c r="D161" s="21"/>
-      <c r="E161" s="20"/>
-      <c r="F161" s="19"/>
+      <c r="A161" s="19"/>
+      <c r="B161" s="19"/>
+      <c r="C161" s="20"/>
+      <c r="D161" s="20"/>
+      <c r="E161" s="19"/>
+      <c r="F161" s="18"/>
       <c r="G161" s="4"/>
       <c r="H161" s="4"/>
       <c r="I161" s="4"/>
@@ -6936,12 +6902,12 @@
       <c r="Z161" s="4"/>
     </row>
     <row r="162" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A162" s="20"/>
-      <c r="B162" s="20"/>
-      <c r="C162" s="21"/>
-      <c r="D162" s="21"/>
-      <c r="E162" s="20"/>
-      <c r="F162" s="19"/>
+      <c r="A162" s="19"/>
+      <c r="B162" s="19"/>
+      <c r="C162" s="20"/>
+      <c r="D162" s="20"/>
+      <c r="E162" s="19"/>
+      <c r="F162" s="18"/>
       <c r="G162" s="4"/>
       <c r="H162" s="4"/>
       <c r="I162" s="4"/>
@@ -6964,12 +6930,12 @@
       <c r="Z162" s="4"/>
     </row>
     <row r="163" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A163" s="20"/>
-      <c r="B163" s="20"/>
-      <c r="C163" s="21"/>
-      <c r="D163" s="21"/>
-      <c r="E163" s="20"/>
-      <c r="F163" s="19"/>
+      <c r="A163" s="19"/>
+      <c r="B163" s="19"/>
+      <c r="C163" s="20"/>
+      <c r="D163" s="20"/>
+      <c r="E163" s="19"/>
+      <c r="F163" s="18"/>
       <c r="G163" s="4"/>
       <c r="H163" s="4"/>
       <c r="I163" s="4"/>
@@ -6992,12 +6958,12 @@
       <c r="Z163" s="4"/>
     </row>
     <row r="164" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A164" s="20"/>
-      <c r="B164" s="20"/>
-      <c r="C164" s="21"/>
-      <c r="D164" s="21"/>
-      <c r="E164" s="20"/>
-      <c r="F164" s="19"/>
+      <c r="A164" s="19"/>
+      <c r="B164" s="19"/>
+      <c r="C164" s="20"/>
+      <c r="D164" s="20"/>
+      <c r="E164" s="19"/>
+      <c r="F164" s="18"/>
       <c r="G164" s="4"/>
       <c r="H164" s="4"/>
       <c r="I164" s="4"/>
@@ -7020,12 +6986,12 @@
       <c r="Z164" s="4"/>
     </row>
     <row r="165" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A165" s="20"/>
-      <c r="B165" s="20"/>
-      <c r="C165" s="21"/>
-      <c r="D165" s="21"/>
-      <c r="E165" s="20"/>
-      <c r="F165" s="19"/>
+      <c r="A165" s="19"/>
+      <c r="B165" s="19"/>
+      <c r="C165" s="20"/>
+      <c r="D165" s="20"/>
+      <c r="E165" s="19"/>
+      <c r="F165" s="18"/>
       <c r="G165" s="4"/>
       <c r="H165" s="4"/>
       <c r="I165" s="4"/>
@@ -7048,12 +7014,12 @@
       <c r="Z165" s="4"/>
     </row>
     <row r="166" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A166" s="20"/>
-      <c r="B166" s="20"/>
-      <c r="C166" s="21"/>
-      <c r="D166" s="21"/>
-      <c r="E166" s="20"/>
-      <c r="F166" s="19"/>
+      <c r="A166" s="19"/>
+      <c r="B166" s="19"/>
+      <c r="C166" s="20"/>
+      <c r="D166" s="20"/>
+      <c r="E166" s="19"/>
+      <c r="F166" s="18"/>
       <c r="G166" s="4"/>
       <c r="H166" s="4"/>
       <c r="I166" s="4"/>
@@ -7076,12 +7042,12 @@
       <c r="Z166" s="4"/>
     </row>
     <row r="167" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A167" s="20"/>
-      <c r="B167" s="20"/>
-      <c r="C167" s="21"/>
-      <c r="D167" s="21"/>
-      <c r="E167" s="20"/>
-      <c r="F167" s="19"/>
+      <c r="A167" s="19"/>
+      <c r="B167" s="19"/>
+      <c r="C167" s="20"/>
+      <c r="D167" s="20"/>
+      <c r="E167" s="19"/>
+      <c r="F167" s="18"/>
       <c r="G167" s="4"/>
       <c r="H167" s="4"/>
       <c r="I167" s="4"/>
@@ -7104,12 +7070,12 @@
       <c r="Z167" s="4"/>
     </row>
     <row r="168" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A168" s="20"/>
-      <c r="B168" s="20"/>
-      <c r="C168" s="19"/>
-      <c r="D168" s="19"/>
-      <c r="E168" s="20"/>
-      <c r="F168" s="17"/>
+      <c r="A168" s="19"/>
+      <c r="B168" s="19"/>
+      <c r="C168" s="18"/>
+      <c r="D168" s="18"/>
+      <c r="E168" s="19"/>
+      <c r="F168" s="16"/>
       <c r="G168" s="4"/>
       <c r="H168" s="4"/>
       <c r="I168" s="4"/>
@@ -7132,12 +7098,12 @@
       <c r="Z168" s="4"/>
     </row>
     <row r="169" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A169" s="20"/>
-      <c r="B169" s="20"/>
-      <c r="C169" s="19"/>
-      <c r="D169" s="19"/>
-      <c r="E169" s="20"/>
-      <c r="F169" s="17"/>
+      <c r="A169" s="19"/>
+      <c r="B169" s="19"/>
+      <c r="C169" s="18"/>
+      <c r="D169" s="18"/>
+      <c r="E169" s="19"/>
+      <c r="F169" s="16"/>
       <c r="G169" s="4"/>
       <c r="H169" s="4"/>
       <c r="I169" s="4"/>
@@ -7160,12 +7126,12 @@
       <c r="Z169" s="4"/>
     </row>
     <row r="170" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A170" s="20"/>
-      <c r="B170" s="20"/>
-      <c r="C170" s="19"/>
-      <c r="D170" s="19"/>
-      <c r="E170" s="20"/>
-      <c r="F170" s="17"/>
+      <c r="A170" s="19"/>
+      <c r="B170" s="19"/>
+      <c r="C170" s="18"/>
+      <c r="D170" s="18"/>
+      <c r="E170" s="19"/>
+      <c r="F170" s="16"/>
       <c r="G170" s="4"/>
       <c r="H170" s="4"/>
       <c r="I170" s="4"/>
@@ -7188,12 +7154,12 @@
       <c r="Z170" s="4"/>
     </row>
     <row r="171" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A171" s="20"/>
-      <c r="B171" s="20"/>
-      <c r="C171" s="21"/>
-      <c r="D171" s="21"/>
-      <c r="E171" s="20"/>
-      <c r="F171" s="19"/>
+      <c r="A171" s="19"/>
+      <c r="B171" s="19"/>
+      <c r="C171" s="20"/>
+      <c r="D171" s="20"/>
+      <c r="E171" s="19"/>
+      <c r="F171" s="18"/>
       <c r="G171" s="4"/>
       <c r="H171" s="4"/>
       <c r="I171" s="4"/>
@@ -7216,12 +7182,12 @@
       <c r="Z171" s="4"/>
     </row>
     <row r="172" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A172" s="20"/>
-      <c r="B172" s="20"/>
-      <c r="C172" s="21"/>
-      <c r="D172" s="21"/>
-      <c r="E172" s="20"/>
-      <c r="F172" s="19"/>
+      <c r="A172" s="19"/>
+      <c r="B172" s="19"/>
+      <c r="C172" s="20"/>
+      <c r="D172" s="20"/>
+      <c r="E172" s="19"/>
+      <c r="F172" s="18"/>
       <c r="G172" s="4"/>
       <c r="H172" s="4"/>
       <c r="I172" s="4"/>
@@ -7244,12 +7210,12 @@
       <c r="Z172" s="4"/>
     </row>
     <row r="173" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A173" s="20"/>
-      <c r="B173" s="20"/>
-      <c r="C173" s="19"/>
-      <c r="D173" s="19"/>
-      <c r="E173" s="20"/>
-      <c r="F173" s="17"/>
+      <c r="A173" s="19"/>
+      <c r="B173" s="19"/>
+      <c r="C173" s="18"/>
+      <c r="D173" s="18"/>
+      <c r="E173" s="19"/>
+      <c r="F173" s="16"/>
       <c r="G173" s="4"/>
       <c r="H173" s="4"/>
       <c r="I173" s="4"/>
@@ -7272,12 +7238,12 @@
       <c r="Z173" s="4"/>
     </row>
     <row r="174" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A174" s="20"/>
-      <c r="B174" s="20"/>
-      <c r="C174" s="19"/>
-      <c r="D174" s="19"/>
-      <c r="E174" s="20"/>
-      <c r="F174" s="17"/>
+      <c r="A174" s="19"/>
+      <c r="B174" s="19"/>
+      <c r="C174" s="18"/>
+      <c r="D174" s="18"/>
+      <c r="E174" s="19"/>
+      <c r="F174" s="16"/>
       <c r="G174" s="4"/>
       <c r="H174" s="4"/>
       <c r="I174" s="4"/>
@@ -7300,12 +7266,12 @@
       <c r="Z174" s="4"/>
     </row>
     <row r="175" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A175" s="20"/>
-      <c r="B175" s="20"/>
-      <c r="C175" s="19"/>
-      <c r="D175" s="19"/>
-      <c r="E175" s="20"/>
-      <c r="F175" s="17"/>
+      <c r="A175" s="19"/>
+      <c r="B175" s="19"/>
+      <c r="C175" s="18"/>
+      <c r="D175" s="18"/>
+      <c r="E175" s="19"/>
+      <c r="F175" s="16"/>
       <c r="G175" s="4"/>
       <c r="H175" s="4"/>
       <c r="I175" s="4"/>
@@ -7328,12 +7294,12 @@
       <c r="Z175" s="4"/>
     </row>
     <row r="176" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A176" s="20"/>
-      <c r="B176" s="20"/>
-      <c r="C176" s="19"/>
-      <c r="D176" s="19"/>
-      <c r="E176" s="20"/>
-      <c r="F176" s="17"/>
+      <c r="A176" s="19"/>
+      <c r="B176" s="19"/>
+      <c r="C176" s="18"/>
+      <c r="D176" s="18"/>
+      <c r="E176" s="19"/>
+      <c r="F176" s="16"/>
       <c r="G176" s="4"/>
       <c r="H176" s="4"/>
       <c r="I176" s="4"/>
@@ -7356,12 +7322,12 @@
       <c r="Z176" s="4"/>
     </row>
     <row r="177" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A177" s="20"/>
-      <c r="B177" s="20"/>
-      <c r="C177" s="19"/>
-      <c r="D177" s="19"/>
-      <c r="E177" s="20"/>
-      <c r="F177" s="17"/>
+      <c r="A177" s="19"/>
+      <c r="B177" s="19"/>
+      <c r="C177" s="18"/>
+      <c r="D177" s="18"/>
+      <c r="E177" s="19"/>
+      <c r="F177" s="16"/>
       <c r="G177" s="4"/>
       <c r="H177" s="4"/>
       <c r="I177" s="4"/>
@@ -7384,12 +7350,12 @@
       <c r="Z177" s="4"/>
     </row>
     <row r="178" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A178" s="20"/>
-      <c r="B178" s="20"/>
-      <c r="C178" s="21"/>
-      <c r="D178" s="21"/>
-      <c r="E178" s="20"/>
-      <c r="F178" s="19"/>
+      <c r="A178" s="19"/>
+      <c r="B178" s="19"/>
+      <c r="C178" s="20"/>
+      <c r="D178" s="20"/>
+      <c r="E178" s="19"/>
+      <c r="F178" s="18"/>
       <c r="G178" s="4"/>
       <c r="H178" s="4"/>
       <c r="I178" s="4"/>
@@ -7412,12 +7378,12 @@
       <c r="Z178" s="4"/>
     </row>
     <row r="179" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A179" s="20"/>
-      <c r="B179" s="20"/>
-      <c r="C179" s="21"/>
-      <c r="D179" s="21"/>
-      <c r="E179" s="20"/>
-      <c r="F179" s="19"/>
+      <c r="A179" s="19"/>
+      <c r="B179" s="19"/>
+      <c r="C179" s="20"/>
+      <c r="D179" s="20"/>
+      <c r="E179" s="19"/>
+      <c r="F179" s="18"/>
       <c r="G179" s="4"/>
       <c r="H179" s="4"/>
       <c r="I179" s="4"/>
@@ -7440,12 +7406,12 @@
       <c r="Z179" s="4"/>
     </row>
     <row r="180" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A180" s="20"/>
-      <c r="B180" s="20"/>
-      <c r="C180" s="19"/>
-      <c r="D180" s="19"/>
-      <c r="E180" s="20"/>
-      <c r="F180" s="19"/>
+      <c r="A180" s="19"/>
+      <c r="B180" s="19"/>
+      <c r="C180" s="18"/>
+      <c r="D180" s="18"/>
+      <c r="E180" s="19"/>
+      <c r="F180" s="18"/>
       <c r="G180" s="4"/>
       <c r="H180" s="4"/>
       <c r="I180" s="4"/>
@@ -7468,12 +7434,12 @@
       <c r="Z180" s="4"/>
     </row>
     <row r="181" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A181" s="20"/>
-      <c r="B181" s="20"/>
-      <c r="C181" s="19"/>
-      <c r="D181" s="19"/>
-      <c r="E181" s="20"/>
-      <c r="F181" s="17"/>
+      <c r="A181" s="19"/>
+      <c r="B181" s="19"/>
+      <c r="C181" s="18"/>
+      <c r="D181" s="18"/>
+      <c r="E181" s="19"/>
+      <c r="F181" s="16"/>
       <c r="G181" s="4"/>
       <c r="H181" s="4"/>
       <c r="I181" s="4"/>
@@ -7496,12 +7462,12 @@
       <c r="Z181" s="4"/>
     </row>
     <row r="182" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A182" s="20"/>
-      <c r="B182" s="20"/>
-      <c r="C182" s="19"/>
-      <c r="D182" s="19"/>
-      <c r="E182" s="20"/>
-      <c r="F182" s="19"/>
+      <c r="A182" s="19"/>
+      <c r="B182" s="19"/>
+      <c r="C182" s="18"/>
+      <c r="D182" s="18"/>
+      <c r="E182" s="19"/>
+      <c r="F182" s="18"/>
       <c r="G182" s="4"/>
       <c r="H182" s="4"/>
       <c r="I182" s="4"/>
@@ -7524,12 +7490,12 @@
       <c r="Z182" s="4"/>
     </row>
     <row r="183" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A183" s="20"/>
-      <c r="B183" s="20"/>
-      <c r="C183" s="19"/>
-      <c r="D183" s="19"/>
-      <c r="E183" s="20"/>
-      <c r="F183" s="17"/>
+      <c r="A183" s="19"/>
+      <c r="B183" s="19"/>
+      <c r="C183" s="18"/>
+      <c r="D183" s="18"/>
+      <c r="E183" s="19"/>
+      <c r="F183" s="16"/>
       <c r="G183" s="4"/>
       <c r="H183" s="4"/>
       <c r="I183" s="4"/>
@@ -7552,12 +7518,12 @@
       <c r="Z183" s="4"/>
     </row>
     <row r="184" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A184" s="20"/>
-      <c r="B184" s="20"/>
-      <c r="C184" s="21"/>
-      <c r="D184" s="21"/>
-      <c r="E184" s="20"/>
-      <c r="F184" s="19"/>
+      <c r="A184" s="19"/>
+      <c r="B184" s="19"/>
+      <c r="C184" s="20"/>
+      <c r="D184" s="20"/>
+      <c r="E184" s="19"/>
+      <c r="F184" s="18"/>
       <c r="G184" s="4"/>
       <c r="H184" s="4"/>
       <c r="I184" s="4"/>
@@ -7580,12 +7546,12 @@
       <c r="Z184" s="4"/>
     </row>
     <row r="185" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A185" s="20"/>
-      <c r="B185" s="20"/>
-      <c r="C185" s="21"/>
-      <c r="D185" s="21"/>
-      <c r="E185" s="20"/>
-      <c r="F185" s="19"/>
+      <c r="A185" s="19"/>
+      <c r="B185" s="19"/>
+      <c r="C185" s="20"/>
+      <c r="D185" s="20"/>
+      <c r="E185" s="19"/>
+      <c r="F185" s="18"/>
       <c r="G185" s="4"/>
       <c r="H185" s="4"/>
       <c r="I185" s="4"/>
@@ -7608,12 +7574,12 @@
       <c r="Z185" s="4"/>
     </row>
     <row r="186" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A186" s="20"/>
-      <c r="B186" s="20"/>
-      <c r="C186" s="21"/>
-      <c r="D186" s="21"/>
-      <c r="E186" s="20"/>
-      <c r="F186" s="19"/>
+      <c r="A186" s="19"/>
+      <c r="B186" s="19"/>
+      <c r="C186" s="20"/>
+      <c r="D186" s="20"/>
+      <c r="E186" s="19"/>
+      <c r="F186" s="18"/>
       <c r="G186" s="4"/>
       <c r="H186" s="4"/>
       <c r="I186" s="4"/>
@@ -7636,12 +7602,12 @@
       <c r="Z186" s="4"/>
     </row>
     <row r="187" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A187" s="20"/>
-      <c r="B187" s="20"/>
-      <c r="C187" s="19"/>
-      <c r="D187" s="19"/>
-      <c r="E187" s="20"/>
-      <c r="F187" s="17"/>
+      <c r="A187" s="19"/>
+      <c r="B187" s="19"/>
+      <c r="C187" s="18"/>
+      <c r="D187" s="18"/>
+      <c r="E187" s="19"/>
+      <c r="F187" s="16"/>
       <c r="G187" s="4"/>
       <c r="H187" s="4"/>
       <c r="I187" s="4"/>
@@ -7664,12 +7630,12 @@
       <c r="Z187" s="4"/>
     </row>
     <row r="188" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A188" s="20"/>
-      <c r="B188" s="20"/>
-      <c r="C188" s="19"/>
-      <c r="D188" s="19"/>
-      <c r="E188" s="20"/>
-      <c r="F188" s="17"/>
+      <c r="A188" s="19"/>
+      <c r="B188" s="19"/>
+      <c r="C188" s="18"/>
+      <c r="D188" s="18"/>
+      <c r="E188" s="19"/>
+      <c r="F188" s="16"/>
       <c r="G188" s="4"/>
       <c r="H188" s="4"/>
       <c r="I188" s="4"/>
@@ -7692,12 +7658,12 @@
       <c r="Z188" s="4"/>
     </row>
     <row r="189" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A189" s="20"/>
-      <c r="B189" s="20"/>
-      <c r="C189" s="19"/>
-      <c r="D189" s="19"/>
-      <c r="E189" s="20"/>
-      <c r="F189" s="17"/>
+      <c r="A189" s="19"/>
+      <c r="B189" s="19"/>
+      <c r="C189" s="18"/>
+      <c r="D189" s="18"/>
+      <c r="E189" s="19"/>
+      <c r="F189" s="16"/>
       <c r="G189" s="4"/>
       <c r="H189" s="4"/>
       <c r="I189" s="4"/>
@@ -7720,12 +7686,12 @@
       <c r="Z189" s="4"/>
     </row>
     <row r="190" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A190" s="20"/>
-      <c r="B190" s="20"/>
-      <c r="C190" s="19"/>
-      <c r="D190" s="19"/>
-      <c r="E190" s="20"/>
-      <c r="F190" s="17"/>
+      <c r="A190" s="19"/>
+      <c r="B190" s="19"/>
+      <c r="C190" s="18"/>
+      <c r="D190" s="18"/>
+      <c r="E190" s="19"/>
+      <c r="F190" s="16"/>
       <c r="G190" s="4"/>
       <c r="H190" s="4"/>
       <c r="I190" s="4"/>
@@ -7748,12 +7714,12 @@
       <c r="Z190" s="4"/>
     </row>
     <row r="191" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A191" s="20"/>
-      <c r="B191" s="20"/>
-      <c r="C191" s="21"/>
-      <c r="D191" s="21"/>
-      <c r="E191" s="20"/>
-      <c r="F191" s="19"/>
+      <c r="A191" s="19"/>
+      <c r="B191" s="19"/>
+      <c r="C191" s="20"/>
+      <c r="D191" s="20"/>
+      <c r="E191" s="19"/>
+      <c r="F191" s="18"/>
       <c r="G191" s="4"/>
       <c r="H191" s="4"/>
       <c r="I191" s="4"/>
@@ -7776,12 +7742,12 @@
       <c r="Z191" s="4"/>
     </row>
     <row r="192" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A192" s="20"/>
-      <c r="B192" s="20"/>
-      <c r="C192" s="21"/>
-      <c r="D192" s="21"/>
-      <c r="E192" s="20"/>
-      <c r="F192" s="19"/>
+      <c r="A192" s="19"/>
+      <c r="B192" s="19"/>
+      <c r="C192" s="20"/>
+      <c r="D192" s="20"/>
+      <c r="E192" s="19"/>
+      <c r="F192" s="18"/>
       <c r="G192" s="4"/>
       <c r="H192" s="4"/>
       <c r="I192" s="4"/>
@@ -7804,12 +7770,12 @@
       <c r="Z192" s="4"/>
     </row>
     <row r="193" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A193" s="20"/>
-      <c r="B193" s="20"/>
-      <c r="C193" s="21"/>
-      <c r="D193" s="21"/>
-      <c r="E193" s="20"/>
-      <c r="F193" s="19"/>
+      <c r="A193" s="19"/>
+      <c r="B193" s="19"/>
+      <c r="C193" s="20"/>
+      <c r="D193" s="20"/>
+      <c r="E193" s="19"/>
+      <c r="F193" s="18"/>
       <c r="G193" s="4"/>
       <c r="H193" s="4"/>
       <c r="I193" s="4"/>
@@ -7832,12 +7798,12 @@
       <c r="Z193" s="4"/>
     </row>
     <row r="194" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A194" s="20"/>
-      <c r="B194" s="20"/>
-      <c r="C194" s="21"/>
-      <c r="D194" s="21"/>
-      <c r="E194" s="20"/>
-      <c r="F194" s="19"/>
+      <c r="A194" s="19"/>
+      <c r="B194" s="19"/>
+      <c r="C194" s="20"/>
+      <c r="D194" s="20"/>
+      <c r="E194" s="19"/>
+      <c r="F194" s="18"/>
       <c r="G194" s="4"/>
       <c r="H194" s="4"/>
       <c r="I194" s="4"/>
@@ -7860,12 +7826,12 @@
       <c r="Z194" s="4"/>
     </row>
     <row r="195" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A195" s="20"/>
-      <c r="B195" s="20"/>
-      <c r="C195" s="21"/>
-      <c r="D195" s="21"/>
-      <c r="E195" s="20"/>
-      <c r="F195" s="19"/>
+      <c r="A195" s="19"/>
+      <c r="B195" s="19"/>
+      <c r="C195" s="20"/>
+      <c r="D195" s="20"/>
+      <c r="E195" s="19"/>
+      <c r="F195" s="18"/>
       <c r="G195" s="4"/>
       <c r="H195" s="4"/>
       <c r="I195" s="4"/>
@@ -7888,12 +7854,12 @@
       <c r="Z195" s="4"/>
     </row>
     <row r="196" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A196" s="20"/>
-      <c r="B196" s="20"/>
-      <c r="C196" s="21"/>
-      <c r="D196" s="21"/>
-      <c r="E196" s="20"/>
-      <c r="F196" s="19"/>
+      <c r="A196" s="19"/>
+      <c r="B196" s="19"/>
+      <c r="C196" s="20"/>
+      <c r="D196" s="20"/>
+      <c r="E196" s="19"/>
+      <c r="F196" s="18"/>
       <c r="G196" s="4"/>
       <c r="H196" s="4"/>
       <c r="I196" s="4"/>
@@ -7916,12 +7882,12 @@
       <c r="Z196" s="4"/>
     </row>
     <row r="197" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A197" s="20"/>
-      <c r="B197" s="20"/>
-      <c r="C197" s="21"/>
-      <c r="D197" s="21"/>
-      <c r="E197" s="20"/>
-      <c r="F197" s="19"/>
+      <c r="A197" s="19"/>
+      <c r="B197" s="19"/>
+      <c r="C197" s="20"/>
+      <c r="D197" s="20"/>
+      <c r="E197" s="19"/>
+      <c r="F197" s="18"/>
       <c r="G197" s="4"/>
       <c r="H197" s="4"/>
       <c r="I197" s="4"/>
@@ -7944,12 +7910,12 @@
       <c r="Z197" s="4"/>
     </row>
     <row r="198" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A198" s="20"/>
-      <c r="B198" s="20"/>
-      <c r="C198" s="21"/>
-      <c r="D198" s="21"/>
-      <c r="E198" s="20"/>
-      <c r="F198" s="19"/>
+      <c r="A198" s="19"/>
+      <c r="B198" s="19"/>
+      <c r="C198" s="20"/>
+      <c r="D198" s="20"/>
+      <c r="E198" s="19"/>
+      <c r="F198" s="18"/>
       <c r="G198" s="4"/>
       <c r="H198" s="4"/>
       <c r="I198" s="4"/>
@@ -7972,12 +7938,12 @@
       <c r="Z198" s="4"/>
     </row>
     <row r="199" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A199" s="20"/>
-      <c r="B199" s="20"/>
-      <c r="C199" s="21"/>
-      <c r="D199" s="21"/>
-      <c r="E199" s="20"/>
-      <c r="F199" s="19"/>
+      <c r="A199" s="19"/>
+      <c r="B199" s="19"/>
+      <c r="C199" s="20"/>
+      <c r="D199" s="20"/>
+      <c r="E199" s="19"/>
+      <c r="F199" s="18"/>
       <c r="G199" s="4"/>
       <c r="H199" s="4"/>
       <c r="I199" s="4"/>
@@ -8000,12 +7966,12 @@
       <c r="Z199" s="4"/>
     </row>
     <row r="200" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A200" s="20"/>
-      <c r="B200" s="20"/>
-      <c r="C200" s="19"/>
-      <c r="D200" s="19"/>
-      <c r="E200" s="20"/>
-      <c r="F200" s="17"/>
+      <c r="A200" s="19"/>
+      <c r="B200" s="19"/>
+      <c r="C200" s="18"/>
+      <c r="D200" s="18"/>
+      <c r="E200" s="19"/>
+      <c r="F200" s="16"/>
       <c r="G200" s="4"/>
       <c r="H200" s="4"/>
       <c r="I200" s="4"/>
@@ -8028,12 +7994,12 @@
       <c r="Z200" s="4"/>
     </row>
     <row r="201" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A201" s="20"/>
-      <c r="B201" s="20"/>
-      <c r="C201" s="19"/>
-      <c r="D201" s="19"/>
-      <c r="E201" s="20"/>
-      <c r="F201" s="17"/>
+      <c r="A201" s="19"/>
+      <c r="B201" s="19"/>
+      <c r="C201" s="18"/>
+      <c r="D201" s="18"/>
+      <c r="E201" s="19"/>
+      <c r="F201" s="16"/>
       <c r="G201" s="4"/>
       <c r="H201" s="4"/>
       <c r="I201" s="4"/>
@@ -8056,12 +8022,12 @@
       <c r="Z201" s="4"/>
     </row>
     <row r="202" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A202" s="20"/>
-      <c r="B202" s="20"/>
-      <c r="C202" s="19"/>
-      <c r="D202" s="19"/>
-      <c r="E202" s="20"/>
-      <c r="F202" s="17"/>
+      <c r="A202" s="19"/>
+      <c r="B202" s="19"/>
+      <c r="C202" s="18"/>
+      <c r="D202" s="18"/>
+      <c r="E202" s="19"/>
+      <c r="F202" s="16"/>
       <c r="G202" s="4"/>
       <c r="H202" s="4"/>
       <c r="I202" s="4"/>
@@ -8084,12 +8050,12 @@
       <c r="Z202" s="4"/>
     </row>
     <row r="203" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A203" s="20"/>
-      <c r="B203" s="20"/>
-      <c r="C203" s="21"/>
-      <c r="D203" s="21"/>
-      <c r="E203" s="20"/>
-      <c r="F203" s="19"/>
+      <c r="A203" s="19"/>
+      <c r="B203" s="19"/>
+      <c r="C203" s="20"/>
+      <c r="D203" s="20"/>
+      <c r="E203" s="19"/>
+      <c r="F203" s="18"/>
       <c r="G203" s="4"/>
       <c r="H203" s="4"/>
       <c r="I203" s="4"/>
@@ -8112,12 +8078,12 @@
       <c r="Z203" s="4"/>
     </row>
     <row r="204" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A204" s="20"/>
-      <c r="B204" s="20"/>
-      <c r="C204" s="21"/>
-      <c r="D204" s="21"/>
-      <c r="E204" s="20"/>
-      <c r="F204" s="19"/>
+      <c r="A204" s="19"/>
+      <c r="B204" s="19"/>
+      <c r="C204" s="20"/>
+      <c r="D204" s="20"/>
+      <c r="E204" s="19"/>
+      <c r="F204" s="18"/>
       <c r="G204" s="4"/>
       <c r="H204" s="4"/>
       <c r="I204" s="4"/>
@@ -8140,12 +8106,12 @@
       <c r="Z204" s="4"/>
     </row>
     <row r="205" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A205" s="20"/>
-      <c r="B205" s="20"/>
-      <c r="C205" s="19"/>
-      <c r="D205" s="19"/>
-      <c r="E205" s="20"/>
-      <c r="F205" s="17"/>
+      <c r="A205" s="19"/>
+      <c r="B205" s="19"/>
+      <c r="C205" s="18"/>
+      <c r="D205" s="18"/>
+      <c r="E205" s="19"/>
+      <c r="F205" s="16"/>
       <c r="G205" s="4"/>
       <c r="H205" s="4"/>
       <c r="I205" s="4"/>
@@ -8168,12 +8134,12 @@
       <c r="Z205" s="4"/>
     </row>
     <row r="206" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A206" s="20"/>
-      <c r="B206" s="20"/>
-      <c r="C206" s="19"/>
-      <c r="D206" s="19"/>
-      <c r="E206" s="20"/>
-      <c r="F206" s="17"/>
+      <c r="A206" s="19"/>
+      <c r="B206" s="19"/>
+      <c r="C206" s="18"/>
+      <c r="D206" s="18"/>
+      <c r="E206" s="19"/>
+      <c r="F206" s="16"/>
       <c r="G206" s="4"/>
       <c r="H206" s="4"/>
       <c r="I206" s="4"/>
@@ -8196,12 +8162,12 @@
       <c r="Z206" s="4"/>
     </row>
     <row r="207" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A207" s="20"/>
-      <c r="B207" s="20"/>
-      <c r="C207" s="19"/>
-      <c r="D207" s="19"/>
-      <c r="E207" s="20"/>
-      <c r="F207" s="19"/>
+      <c r="A207" s="19"/>
+      <c r="B207" s="19"/>
+      <c r="C207" s="18"/>
+      <c r="D207" s="18"/>
+      <c r="E207" s="19"/>
+      <c r="F207" s="18"/>
       <c r="G207" s="4"/>
       <c r="H207" s="4"/>
       <c r="I207" s="4"/>
@@ -8224,12 +8190,12 @@
       <c r="Z207" s="4"/>
     </row>
     <row r="208" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A208" s="20"/>
-      <c r="B208" s="20"/>
-      <c r="C208" s="19"/>
-      <c r="D208" s="19"/>
-      <c r="E208" s="20"/>
-      <c r="F208" s="19"/>
+      <c r="A208" s="19"/>
+      <c r="B208" s="19"/>
+      <c r="C208" s="18"/>
+      <c r="D208" s="18"/>
+      <c r="E208" s="19"/>
+      <c r="F208" s="18"/>
       <c r="G208" s="4"/>
       <c r="H208" s="4"/>
       <c r="I208" s="4"/>
@@ -8252,12 +8218,12 @@
       <c r="Z208" s="4"/>
     </row>
     <row r="209" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A209" s="20"/>
-      <c r="B209" s="20"/>
-      <c r="C209" s="19"/>
-      <c r="D209" s="19"/>
-      <c r="E209" s="20"/>
-      <c r="F209" s="17"/>
+      <c r="A209" s="19"/>
+      <c r="B209" s="19"/>
+      <c r="C209" s="18"/>
+      <c r="D209" s="18"/>
+      <c r="E209" s="19"/>
+      <c r="F209" s="16"/>
       <c r="G209" s="4"/>
       <c r="H209" s="4"/>
       <c r="I209" s="4"/>
@@ -8280,12 +8246,12 @@
       <c r="Z209" s="4"/>
     </row>
     <row r="210" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A210" s="20"/>
-      <c r="B210" s="20"/>
-      <c r="C210" s="19"/>
-      <c r="D210" s="19"/>
-      <c r="E210" s="20"/>
-      <c r="F210" s="17"/>
+      <c r="A210" s="19"/>
+      <c r="B210" s="19"/>
+      <c r="C210" s="18"/>
+      <c r="D210" s="18"/>
+      <c r="E210" s="19"/>
+      <c r="F210" s="16"/>
       <c r="G210" s="4"/>
       <c r="H210" s="4"/>
       <c r="I210" s="4"/>
@@ -8308,12 +8274,12 @@
       <c r="Z210" s="4"/>
     </row>
     <row r="211" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A211" s="20"/>
-      <c r="B211" s="20"/>
-      <c r="C211" s="19"/>
-      <c r="D211" s="19"/>
-      <c r="E211" s="20"/>
-      <c r="F211" s="17"/>
+      <c r="A211" s="19"/>
+      <c r="B211" s="19"/>
+      <c r="C211" s="18"/>
+      <c r="D211" s="18"/>
+      <c r="E211" s="19"/>
+      <c r="F211" s="16"/>
       <c r="G211" s="4"/>
       <c r="H211" s="4"/>
       <c r="I211" s="4"/>
@@ -8336,12 +8302,12 @@
       <c r="Z211" s="4"/>
     </row>
     <row r="212" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A212" s="20"/>
-      <c r="B212" s="20"/>
-      <c r="C212" s="19"/>
-      <c r="D212" s="19"/>
-      <c r="E212" s="20"/>
-      <c r="F212" s="17"/>
+      <c r="A212" s="19"/>
+      <c r="B212" s="19"/>
+      <c r="C212" s="18"/>
+      <c r="D212" s="18"/>
+      <c r="E212" s="19"/>
+      <c r="F212" s="16"/>
       <c r="G212" s="4"/>
       <c r="H212" s="4"/>
       <c r="I212" s="4"/>
@@ -8364,12 +8330,12 @@
       <c r="Z212" s="4"/>
     </row>
     <row r="213" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A213" s="20"/>
-      <c r="B213" s="20"/>
-      <c r="C213" s="19"/>
-      <c r="D213" s="19"/>
-      <c r="E213" s="20"/>
-      <c r="F213" s="17"/>
+      <c r="A213" s="19"/>
+      <c r="B213" s="19"/>
+      <c r="C213" s="18"/>
+      <c r="D213" s="18"/>
+      <c r="E213" s="19"/>
+      <c r="F213" s="16"/>
       <c r="G213" s="4"/>
       <c r="H213" s="4"/>
       <c r="I213" s="4"/>
@@ -8392,12 +8358,12 @@
       <c r="Z213" s="4"/>
     </row>
     <row r="214" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A214" s="20"/>
-      <c r="B214" s="20"/>
-      <c r="C214" s="21"/>
-      <c r="D214" s="21"/>
-      <c r="E214" s="20"/>
-      <c r="F214" s="19"/>
+      <c r="A214" s="19"/>
+      <c r="B214" s="19"/>
+      <c r="C214" s="20"/>
+      <c r="D214" s="20"/>
+      <c r="E214" s="19"/>
+      <c r="F214" s="18"/>
       <c r="G214" s="4"/>
       <c r="H214" s="4"/>
       <c r="I214" s="4"/>
@@ -8420,12 +8386,12 @@
       <c r="Z214" s="4"/>
     </row>
     <row r="215" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A215" s="20"/>
-      <c r="B215" s="20"/>
-      <c r="C215" s="21"/>
-      <c r="D215" s="21"/>
-      <c r="E215" s="20"/>
-      <c r="F215" s="19"/>
+      <c r="A215" s="19"/>
+      <c r="B215" s="19"/>
+      <c r="C215" s="20"/>
+      <c r="D215" s="20"/>
+      <c r="E215" s="19"/>
+      <c r="F215" s="18"/>
       <c r="G215" s="4"/>
       <c r="H215" s="4"/>
       <c r="I215" s="4"/>
@@ -8448,12 +8414,12 @@
       <c r="Z215" s="4"/>
     </row>
     <row r="216" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A216" s="20"/>
-      <c r="B216" s="20"/>
-      <c r="C216" s="19"/>
-      <c r="D216" s="19"/>
-      <c r="E216" s="20"/>
-      <c r="F216" s="17"/>
+      <c r="A216" s="19"/>
+      <c r="B216" s="19"/>
+      <c r="C216" s="18"/>
+      <c r="D216" s="18"/>
+      <c r="E216" s="19"/>
+      <c r="F216" s="16"/>
       <c r="G216" s="4"/>
       <c r="H216" s="4"/>
       <c r="I216" s="4"/>
@@ -8476,12 +8442,12 @@
       <c r="Z216" s="4"/>
     </row>
     <row r="217" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A217" s="20"/>
-      <c r="B217" s="20"/>
-      <c r="C217" s="19"/>
-      <c r="D217" s="19"/>
-      <c r="E217" s="20"/>
-      <c r="F217" s="17"/>
+      <c r="A217" s="19"/>
+      <c r="B217" s="19"/>
+      <c r="C217" s="18"/>
+      <c r="D217" s="18"/>
+      <c r="E217" s="19"/>
+      <c r="F217" s="16"/>
       <c r="G217" s="4"/>
       <c r="H217" s="4"/>
       <c r="I217" s="4"/>
@@ -8504,12 +8470,12 @@
       <c r="Z217" s="4"/>
     </row>
     <row r="218" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A218" s="20"/>
-      <c r="B218" s="20"/>
-      <c r="C218" s="21"/>
-      <c r="D218" s="21"/>
-      <c r="E218" s="20"/>
-      <c r="F218" s="19"/>
+      <c r="A218" s="19"/>
+      <c r="B218" s="19"/>
+      <c r="C218" s="20"/>
+      <c r="D218" s="20"/>
+      <c r="E218" s="19"/>
+      <c r="F218" s="18"/>
       <c r="G218" s="4"/>
       <c r="H218" s="4"/>
       <c r="I218" s="4"/>
@@ -8532,12 +8498,12 @@
       <c r="Z218" s="4"/>
     </row>
     <row r="219" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A219" s="20"/>
-      <c r="B219" s="20"/>
-      <c r="C219" s="21"/>
-      <c r="D219" s="21"/>
-      <c r="E219" s="20"/>
-      <c r="F219" s="19"/>
+      <c r="A219" s="19"/>
+      <c r="B219" s="19"/>
+      <c r="C219" s="20"/>
+      <c r="D219" s="20"/>
+      <c r="E219" s="19"/>
+      <c r="F219" s="18"/>
       <c r="G219" s="4"/>
       <c r="H219" s="4"/>
       <c r="I219" s="4"/>
@@ -8560,12 +8526,12 @@
       <c r="Z219" s="4"/>
     </row>
     <row r="220" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A220" s="20"/>
-      <c r="B220" s="20"/>
-      <c r="C220" s="21"/>
-      <c r="D220" s="21"/>
-      <c r="E220" s="20"/>
-      <c r="F220" s="19"/>
+      <c r="A220" s="19"/>
+      <c r="B220" s="19"/>
+      <c r="C220" s="20"/>
+      <c r="D220" s="20"/>
+      <c r="E220" s="19"/>
+      <c r="F220" s="18"/>
       <c r="G220" s="4"/>
       <c r="H220" s="4"/>
       <c r="I220" s="4"/>
@@ -8588,12 +8554,12 @@
       <c r="Z220" s="4"/>
     </row>
     <row r="221" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A221" s="20"/>
-      <c r="B221" s="20"/>
-      <c r="C221" s="21"/>
-      <c r="D221" s="21"/>
-      <c r="E221" s="20"/>
-      <c r="F221" s="19"/>
+      <c r="A221" s="19"/>
+      <c r="B221" s="19"/>
+      <c r="C221" s="20"/>
+      <c r="D221" s="20"/>
+      <c r="E221" s="19"/>
+      <c r="F221" s="18"/>
       <c r="G221" s="4"/>
       <c r="H221" s="4"/>
       <c r="I221" s="4"/>
@@ -8616,12 +8582,12 @@
       <c r="Z221" s="4"/>
     </row>
     <row r="222" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A222" s="20"/>
-      <c r="B222" s="20"/>
-      <c r="C222" s="19"/>
-      <c r="D222" s="19"/>
-      <c r="E222" s="20"/>
-      <c r="F222" s="17"/>
+      <c r="A222" s="19"/>
+      <c r="B222" s="19"/>
+      <c r="C222" s="18"/>
+      <c r="D222" s="18"/>
+      <c r="E222" s="19"/>
+      <c r="F222" s="16"/>
       <c r="G222" s="4"/>
       <c r="H222" s="4"/>
       <c r="I222" s="4"/>
@@ -8644,12 +8610,12 @@
       <c r="Z222" s="4"/>
     </row>
     <row r="223" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A223" s="20"/>
-      <c r="B223" s="20"/>
-      <c r="C223" s="21"/>
-      <c r="D223" s="21"/>
-      <c r="E223" s="20"/>
-      <c r="F223" s="19"/>
+      <c r="A223" s="19"/>
+      <c r="B223" s="19"/>
+      <c r="C223" s="20"/>
+      <c r="D223" s="20"/>
+      <c r="E223" s="19"/>
+      <c r="F223" s="18"/>
       <c r="G223" s="4"/>
       <c r="H223" s="4"/>
       <c r="I223" s="4"/>
@@ -8672,12 +8638,12 @@
       <c r="Z223" s="4"/>
     </row>
     <row r="224" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A224" s="20"/>
-      <c r="B224" s="20"/>
-      <c r="C224" s="21"/>
-      <c r="D224" s="21"/>
-      <c r="E224" s="20"/>
-      <c r="F224" s="19"/>
+      <c r="A224" s="19"/>
+      <c r="B224" s="19"/>
+      <c r="C224" s="20"/>
+      <c r="D224" s="20"/>
+      <c r="E224" s="19"/>
+      <c r="F224" s="18"/>
       <c r="G224" s="4"/>
       <c r="H224" s="4"/>
       <c r="I224" s="4"/>
@@ -8700,12 +8666,12 @@
       <c r="Z224" s="4"/>
     </row>
     <row r="225" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A225" s="20"/>
-      <c r="B225" s="20"/>
-      <c r="C225" s="21"/>
-      <c r="D225" s="21"/>
-      <c r="E225" s="20"/>
-      <c r="F225" s="19"/>
+      <c r="A225" s="19"/>
+      <c r="B225" s="19"/>
+      <c r="C225" s="20"/>
+      <c r="D225" s="20"/>
+      <c r="E225" s="19"/>
+      <c r="F225" s="18"/>
       <c r="G225" s="4"/>
       <c r="H225" s="4"/>
       <c r="I225" s="4"/>
@@ -8728,12 +8694,12 @@
       <c r="Z225" s="4"/>
     </row>
     <row r="226" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A226" s="20"/>
-      <c r="B226" s="20"/>
-      <c r="C226" s="19"/>
-      <c r="D226" s="19"/>
-      <c r="E226" s="20"/>
-      <c r="F226" s="17"/>
+      <c r="A226" s="19"/>
+      <c r="B226" s="19"/>
+      <c r="C226" s="18"/>
+      <c r="D226" s="18"/>
+      <c r="E226" s="19"/>
+      <c r="F226" s="16"/>
       <c r="G226" s="4"/>
       <c r="H226" s="4"/>
       <c r="I226" s="4"/>
@@ -8756,12 +8722,12 @@
       <c r="Z226" s="4"/>
     </row>
     <row r="227" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A227" s="20"/>
-      <c r="B227" s="20"/>
-      <c r="C227" s="21"/>
-      <c r="D227" s="21"/>
-      <c r="E227" s="20"/>
-      <c r="F227" s="19"/>
+      <c r="A227" s="19"/>
+      <c r="B227" s="19"/>
+      <c r="C227" s="20"/>
+      <c r="D227" s="20"/>
+      <c r="E227" s="19"/>
+      <c r="F227" s="18"/>
       <c r="G227" s="4"/>
       <c r="H227" s="4"/>
       <c r="I227" s="4"/>
@@ -8784,12 +8750,12 @@
       <c r="Z227" s="4"/>
     </row>
     <row r="228" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A228" s="20"/>
-      <c r="B228" s="20"/>
-      <c r="C228" s="21"/>
-      <c r="D228" s="21"/>
-      <c r="E228" s="20"/>
-      <c r="F228" s="19"/>
+      <c r="A228" s="19"/>
+      <c r="B228" s="19"/>
+      <c r="C228" s="20"/>
+      <c r="D228" s="20"/>
+      <c r="E228" s="19"/>
+      <c r="F228" s="18"/>
       <c r="G228" s="4"/>
       <c r="H228" s="4"/>
       <c r="I228" s="4"/>
@@ -8812,12 +8778,12 @@
       <c r="Z228" s="4"/>
     </row>
     <row r="229" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A229" s="20"/>
-      <c r="B229" s="20"/>
-      <c r="C229" s="21"/>
-      <c r="D229" s="21"/>
-      <c r="E229" s="20"/>
-      <c r="F229" s="19"/>
+      <c r="A229" s="19"/>
+      <c r="B229" s="19"/>
+      <c r="C229" s="20"/>
+      <c r="D229" s="20"/>
+      <c r="E229" s="19"/>
+      <c r="F229" s="18"/>
       <c r="G229" s="4"/>
       <c r="H229" s="4"/>
       <c r="I229" s="4"/>
@@ -8840,12 +8806,12 @@
       <c r="Z229" s="4"/>
     </row>
     <row r="230" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A230" s="20"/>
-      <c r="B230" s="20"/>
-      <c r="C230" s="21"/>
-      <c r="D230" s="21"/>
-      <c r="E230" s="20"/>
-      <c r="F230" s="19"/>
+      <c r="A230" s="19"/>
+      <c r="B230" s="19"/>
+      <c r="C230" s="20"/>
+      <c r="D230" s="20"/>
+      <c r="E230" s="19"/>
+      <c r="F230" s="18"/>
       <c r="G230" s="4"/>
       <c r="H230" s="4"/>
       <c r="I230" s="4"/>
@@ -8868,12 +8834,12 @@
       <c r="Z230" s="4"/>
     </row>
     <row r="231" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A231" s="20"/>
-      <c r="B231" s="20"/>
-      <c r="C231" s="21"/>
-      <c r="D231" s="21"/>
-      <c r="E231" s="20"/>
-      <c r="F231" s="19"/>
+      <c r="A231" s="19"/>
+      <c r="B231" s="19"/>
+      <c r="C231" s="20"/>
+      <c r="D231" s="20"/>
+      <c r="E231" s="19"/>
+      <c r="F231" s="18"/>
       <c r="G231" s="4"/>
       <c r="H231" s="4"/>
       <c r="I231" s="4"/>
@@ -8896,12 +8862,12 @@
       <c r="Z231" s="4"/>
     </row>
     <row r="232" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A232" s="20"/>
-      <c r="B232" s="20"/>
-      <c r="C232" s="21"/>
-      <c r="D232" s="21"/>
-      <c r="E232" s="20"/>
-      <c r="F232" s="19"/>
+      <c r="A232" s="19"/>
+      <c r="B232" s="19"/>
+      <c r="C232" s="20"/>
+      <c r="D232" s="20"/>
+      <c r="E232" s="19"/>
+      <c r="F232" s="18"/>
       <c r="G232" s="4"/>
       <c r="H232" s="4"/>
       <c r="I232" s="4"/>
@@ -8924,12 +8890,12 @@
       <c r="Z232" s="4"/>
     </row>
     <row r="233" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A233" s="20"/>
-      <c r="B233" s="20"/>
-      <c r="C233" s="21"/>
-      <c r="D233" s="21"/>
-      <c r="E233" s="20"/>
-      <c r="F233" s="19"/>
+      <c r="A233" s="19"/>
+      <c r="B233" s="19"/>
+      <c r="C233" s="20"/>
+      <c r="D233" s="20"/>
+      <c r="E233" s="19"/>
+      <c r="F233" s="18"/>
       <c r="G233" s="4"/>
       <c r="H233" s="4"/>
       <c r="I233" s="4"/>
@@ -8952,12 +8918,12 @@
       <c r="Z233" s="4"/>
     </row>
     <row r="234" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A234" s="20"/>
-      <c r="B234" s="20"/>
-      <c r="C234" s="19"/>
-      <c r="D234" s="19"/>
-      <c r="E234" s="20"/>
-      <c r="F234" s="17"/>
+      <c r="A234" s="19"/>
+      <c r="B234" s="19"/>
+      <c r="C234" s="18"/>
+      <c r="D234" s="18"/>
+      <c r="E234" s="19"/>
+      <c r="F234" s="16"/>
       <c r="G234" s="4"/>
       <c r="H234" s="4"/>
       <c r="I234" s="4"/>
@@ -8980,12 +8946,12 @@
       <c r="Z234" s="4"/>
     </row>
     <row r="235" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A235" s="20"/>
-      <c r="B235" s="20"/>
-      <c r="C235" s="19"/>
-      <c r="D235" s="19"/>
-      <c r="E235" s="20"/>
-      <c r="F235" s="17"/>
+      <c r="A235" s="19"/>
+      <c r="B235" s="19"/>
+      <c r="C235" s="18"/>
+      <c r="D235" s="18"/>
+      <c r="E235" s="19"/>
+      <c r="F235" s="16"/>
       <c r="G235" s="4"/>
       <c r="H235" s="4"/>
       <c r="I235" s="4"/>
@@ -9008,12 +8974,12 @@
       <c r="Z235" s="4"/>
     </row>
     <row r="236" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A236" s="20"/>
-      <c r="B236" s="20"/>
-      <c r="C236" s="19"/>
-      <c r="D236" s="19"/>
-      <c r="E236" s="20"/>
-      <c r="F236" s="19"/>
+      <c r="A236" s="19"/>
+      <c r="B236" s="19"/>
+      <c r="C236" s="18"/>
+      <c r="D236" s="18"/>
+      <c r="E236" s="19"/>
+      <c r="F236" s="18"/>
       <c r="G236" s="4"/>
       <c r="H236" s="4"/>
       <c r="I236" s="4"/>
@@ -9036,12 +9002,12 @@
       <c r="Z236" s="4"/>
     </row>
     <row r="237" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A237" s="20"/>
-      <c r="B237" s="20"/>
-      <c r="C237" s="19"/>
-      <c r="D237" s="19"/>
-      <c r="E237" s="20"/>
-      <c r="F237" s="17"/>
+      <c r="A237" s="19"/>
+      <c r="B237" s="19"/>
+      <c r="C237" s="18"/>
+      <c r="D237" s="18"/>
+      <c r="E237" s="19"/>
+      <c r="F237" s="16"/>
       <c r="G237" s="4"/>
       <c r="H237" s="4"/>
       <c r="I237" s="4"/>
@@ -9064,12 +9030,12 @@
       <c r="Z237" s="4"/>
     </row>
     <row r="238" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A238" s="20"/>
-      <c r="B238" s="20"/>
-      <c r="C238" s="21"/>
-      <c r="D238" s="21"/>
-      <c r="E238" s="20"/>
-      <c r="F238" s="19"/>
+      <c r="A238" s="19"/>
+      <c r="B238" s="19"/>
+      <c r="C238" s="20"/>
+      <c r="D238" s="20"/>
+      <c r="E238" s="19"/>
+      <c r="F238" s="18"/>
       <c r="G238" s="4"/>
       <c r="H238" s="4"/>
       <c r="I238" s="4"/>
@@ -9092,12 +9058,12 @@
       <c r="Z238" s="4"/>
     </row>
     <row r="239" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A239" s="20"/>
-      <c r="B239" s="20"/>
-      <c r="C239" s="19"/>
-      <c r="D239" s="19"/>
-      <c r="E239" s="20"/>
-      <c r="F239" s="17"/>
+      <c r="A239" s="19"/>
+      <c r="B239" s="19"/>
+      <c r="C239" s="18"/>
+      <c r="D239" s="18"/>
+      <c r="E239" s="19"/>
+      <c r="F239" s="16"/>
       <c r="G239" s="4"/>
       <c r="H239" s="4"/>
       <c r="I239" s="4"/>
@@ -9120,12 +9086,12 @@
       <c r="Z239" s="4"/>
     </row>
     <row r="240" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A240" s="20"/>
-      <c r="B240" s="20"/>
-      <c r="C240" s="19"/>
-      <c r="D240" s="19"/>
-      <c r="E240" s="20"/>
-      <c r="F240" s="17"/>
+      <c r="A240" s="19"/>
+      <c r="B240" s="19"/>
+      <c r="C240" s="18"/>
+      <c r="D240" s="18"/>
+      <c r="E240" s="19"/>
+      <c r="F240" s="16"/>
       <c r="G240" s="4"/>
       <c r="H240" s="4"/>
       <c r="I240" s="4"/>
@@ -9148,12 +9114,12 @@
       <c r="Z240" s="4"/>
     </row>
     <row r="241" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A241" s="20"/>
-      <c r="B241" s="20"/>
-      <c r="C241" s="19"/>
-      <c r="D241" s="19"/>
-      <c r="E241" s="20"/>
-      <c r="F241" s="17"/>
+      <c r="A241" s="19"/>
+      <c r="B241" s="19"/>
+      <c r="C241" s="18"/>
+      <c r="D241" s="18"/>
+      <c r="E241" s="19"/>
+      <c r="F241" s="16"/>
       <c r="G241" s="4"/>
       <c r="H241" s="4"/>
       <c r="I241" s="4"/>
@@ -9176,12 +9142,12 @@
       <c r="Z241" s="4"/>
     </row>
     <row r="242" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A242" s="20"/>
-      <c r="B242" s="20"/>
-      <c r="C242" s="19"/>
-      <c r="D242" s="19"/>
-      <c r="E242" s="20"/>
-      <c r="F242" s="17"/>
+      <c r="A242" s="19"/>
+      <c r="B242" s="19"/>
+      <c r="C242" s="18"/>
+      <c r="D242" s="18"/>
+      <c r="E242" s="19"/>
+      <c r="F242" s="16"/>
       <c r="G242" s="4"/>
       <c r="H242" s="4"/>
       <c r="I242" s="4"/>
@@ -9204,12 +9170,12 @@
       <c r="Z242" s="4"/>
     </row>
     <row r="243" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A243" s="20"/>
-      <c r="B243" s="20"/>
-      <c r="C243" s="19"/>
-      <c r="D243" s="19"/>
-      <c r="E243" s="20"/>
-      <c r="F243" s="17"/>
+      <c r="A243" s="19"/>
+      <c r="B243" s="19"/>
+      <c r="C243" s="18"/>
+      <c r="D243" s="18"/>
+      <c r="E243" s="19"/>
+      <c r="F243" s="16"/>
       <c r="G243" s="4"/>
       <c r="H243" s="4"/>
       <c r="I243" s="4"/>
@@ -9232,12 +9198,12 @@
       <c r="Z243" s="4"/>
     </row>
     <row r="244" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A244" s="20"/>
-      <c r="B244" s="20"/>
-      <c r="C244" s="19"/>
-      <c r="D244" s="19"/>
-      <c r="E244" s="20"/>
-      <c r="F244" s="17"/>
+      <c r="A244" s="19"/>
+      <c r="B244" s="19"/>
+      <c r="C244" s="18"/>
+      <c r="D244" s="18"/>
+      <c r="E244" s="19"/>
+      <c r="F244" s="16"/>
       <c r="G244" s="4"/>
       <c r="H244" s="4"/>
       <c r="I244" s="4"/>
@@ -9260,12 +9226,12 @@
       <c r="Z244" s="4"/>
     </row>
     <row r="245" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A245" s="20"/>
-      <c r="B245" s="20"/>
-      <c r="C245" s="19"/>
-      <c r="D245" s="19"/>
-      <c r="E245" s="20"/>
-      <c r="F245" s="17"/>
+      <c r="A245" s="19"/>
+      <c r="B245" s="19"/>
+      <c r="C245" s="18"/>
+      <c r="D245" s="18"/>
+      <c r="E245" s="19"/>
+      <c r="F245" s="16"/>
       <c r="G245" s="4"/>
       <c r="H245" s="4"/>
       <c r="I245" s="4"/>
@@ -9288,12 +9254,12 @@
       <c r="Z245" s="4"/>
     </row>
     <row r="246" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A246" s="20"/>
-      <c r="B246" s="20"/>
-      <c r="C246" s="19"/>
-      <c r="D246" s="19"/>
-      <c r="E246" s="20"/>
-      <c r="F246" s="17"/>
+      <c r="A246" s="19"/>
+      <c r="B246" s="19"/>
+      <c r="C246" s="18"/>
+      <c r="D246" s="18"/>
+      <c r="E246" s="19"/>
+      <c r="F246" s="16"/>
       <c r="G246" s="4"/>
       <c r="H246" s="4"/>
       <c r="I246" s="4"/>
@@ -9316,12 +9282,12 @@
       <c r="Z246" s="4"/>
     </row>
     <row r="247" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A247" s="20"/>
-      <c r="B247" s="20"/>
-      <c r="C247" s="19"/>
-      <c r="D247" s="19"/>
-      <c r="E247" s="20"/>
-      <c r="F247" s="17"/>
+      <c r="A247" s="19"/>
+      <c r="B247" s="19"/>
+      <c r="C247" s="18"/>
+      <c r="D247" s="18"/>
+      <c r="E247" s="19"/>
+      <c r="F247" s="16"/>
       <c r="G247" s="4"/>
       <c r="H247" s="4"/>
       <c r="I247" s="4"/>
@@ -9344,12 +9310,12 @@
       <c r="Z247" s="4"/>
     </row>
     <row r="248" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A248" s="20"/>
-      <c r="B248" s="20"/>
-      <c r="C248" s="19"/>
-      <c r="D248" s="19"/>
-      <c r="E248" s="20"/>
-      <c r="F248" s="17"/>
+      <c r="A248" s="19"/>
+      <c r="B248" s="19"/>
+      <c r="C248" s="18"/>
+      <c r="D248" s="18"/>
+      <c r="E248" s="19"/>
+      <c r="F248" s="16"/>
       <c r="G248" s="4"/>
       <c r="H248" s="4"/>
       <c r="I248" s="4"/>
@@ -9372,12 +9338,12 @@
       <c r="Z248" s="4"/>
     </row>
     <row r="249" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A249" s="20"/>
-      <c r="B249" s="20"/>
-      <c r="C249" s="19"/>
-      <c r="D249" s="19"/>
-      <c r="E249" s="20"/>
-      <c r="F249" s="17"/>
+      <c r="A249" s="19"/>
+      <c r="B249" s="19"/>
+      <c r="C249" s="18"/>
+      <c r="D249" s="18"/>
+      <c r="E249" s="19"/>
+      <c r="F249" s="16"/>
       <c r="G249" s="4"/>
       <c r="H249" s="4"/>
       <c r="I249" s="4"/>
@@ -9400,12 +9366,12 @@
       <c r="Z249" s="4"/>
     </row>
     <row r="250" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A250" s="20"/>
-      <c r="B250" s="20"/>
-      <c r="C250" s="19"/>
-      <c r="D250" s="19"/>
-      <c r="E250" s="20"/>
-      <c r="F250" s="17"/>
+      <c r="A250" s="19"/>
+      <c r="B250" s="19"/>
+      <c r="C250" s="18"/>
+      <c r="D250" s="18"/>
+      <c r="E250" s="19"/>
+      <c r="F250" s="16"/>
       <c r="G250" s="4"/>
       <c r="H250" s="4"/>
       <c r="I250" s="4"/>
@@ -9428,12 +9394,12 @@
       <c r="Z250" s="4"/>
     </row>
     <row r="251" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A251" s="20"/>
-      <c r="B251" s="20"/>
-      <c r="C251" s="19"/>
-      <c r="D251" s="19"/>
-      <c r="E251" s="20"/>
-      <c r="F251" s="17"/>
+      <c r="A251" s="19"/>
+      <c r="B251" s="19"/>
+      <c r="C251" s="18"/>
+      <c r="D251" s="18"/>
+      <c r="E251" s="19"/>
+      <c r="F251" s="16"/>
       <c r="G251" s="4"/>
       <c r="H251" s="4"/>
       <c r="I251" s="4"/>
@@ -9456,12 +9422,12 @@
       <c r="Z251" s="4"/>
     </row>
     <row r="252" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A252" s="20"/>
-      <c r="B252" s="20"/>
-      <c r="C252" s="19"/>
-      <c r="D252" s="19"/>
-      <c r="E252" s="20"/>
-      <c r="F252" s="17"/>
+      <c r="A252" s="19"/>
+      <c r="B252" s="19"/>
+      <c r="C252" s="18"/>
+      <c r="D252" s="18"/>
+      <c r="E252" s="19"/>
+      <c r="F252" s="16"/>
       <c r="G252" s="4"/>
       <c r="H252" s="4"/>
       <c r="I252" s="4"/>
@@ -9484,12 +9450,12 @@
       <c r="Z252" s="4"/>
     </row>
     <row r="253" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A253" s="20"/>
-      <c r="B253" s="20"/>
-      <c r="C253" s="19"/>
-      <c r="D253" s="19"/>
-      <c r="E253" s="20"/>
-      <c r="F253" s="17"/>
+      <c r="A253" s="19"/>
+      <c r="B253" s="19"/>
+      <c r="C253" s="18"/>
+      <c r="D253" s="18"/>
+      <c r="E253" s="19"/>
+      <c r="F253" s="16"/>
       <c r="G253" s="4"/>
       <c r="H253" s="4"/>
       <c r="I253" s="4"/>
@@ -9512,12 +9478,12 @@
       <c r="Z253" s="4"/>
     </row>
     <row r="254" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A254" s="20"/>
-      <c r="B254" s="20"/>
-      <c r="C254" s="19"/>
-      <c r="D254" s="19"/>
-      <c r="E254" s="20"/>
-      <c r="F254" s="17"/>
+      <c r="A254" s="19"/>
+      <c r="B254" s="19"/>
+      <c r="C254" s="18"/>
+      <c r="D254" s="18"/>
+      <c r="E254" s="19"/>
+      <c r="F254" s="16"/>
       <c r="G254" s="4"/>
       <c r="H254" s="4"/>
       <c r="I254" s="4"/>
@@ -9540,12 +9506,12 @@
       <c r="Z254" s="4"/>
     </row>
     <row r="255" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A255" s="20"/>
-      <c r="B255" s="20"/>
-      <c r="C255" s="19"/>
-      <c r="D255" s="19"/>
-      <c r="E255" s="20"/>
-      <c r="F255" s="17"/>
+      <c r="A255" s="19"/>
+      <c r="B255" s="19"/>
+      <c r="C255" s="18"/>
+      <c r="D255" s="18"/>
+      <c r="E255" s="19"/>
+      <c r="F255" s="16"/>
       <c r="G255" s="4"/>
       <c r="H255" s="4"/>
       <c r="I255" s="4"/>
@@ -9568,12 +9534,12 @@
       <c r="Z255" s="4"/>
     </row>
     <row r="256" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A256" s="20"/>
-      <c r="B256" s="20"/>
-      <c r="C256" s="19"/>
-      <c r="D256" s="19"/>
-      <c r="E256" s="20"/>
-      <c r="F256" s="17"/>
+      <c r="A256" s="19"/>
+      <c r="B256" s="19"/>
+      <c r="C256" s="18"/>
+      <c r="D256" s="18"/>
+      <c r="E256" s="19"/>
+      <c r="F256" s="16"/>
       <c r="G256" s="4"/>
       <c r="H256" s="4"/>
       <c r="I256" s="4"/>
@@ -30518,7 +30484,6 @@
     <hyperlink ref="F41" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
     <hyperlink ref="F42" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
     <hyperlink ref="F44" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="C47" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>

</xml_diff>